<commit_message>
final updates to initia schedule and calendar
</commit_message>
<xml_diff>
--- a/CS320-Spring2020Calendar.xlsx
+++ b/CS320-Spring2020Calendar.xlsx
@@ -89,24 +89,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Lecture 2:
-HTML &amp; CSS
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Lab 1: HTML and CSS assigned</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Lecture 13: Relational Databases
 </t>
     </r>
@@ -281,9 +263,6 @@
 A11: Team Project
 Final Self/Peer Evaluations due
 both 7:00 am (Marmoset)</t>
-  </si>
-  <si>
-    <t>A06: Domain Analysis due</t>
   </si>
   <si>
     <r>
@@ -331,52 +310,7 @@
     <t>Work Ethic Lecture</t>
   </si>
   <si>
-    <t>CS320: SW Engineering - Spring 2020 Schedule
-(as of 1-14-2020, subject to change)</t>
-  </si>
-  <si>
     <t>Final Presentation &amp; Demo</t>
-  </si>
-  <si>
-    <t>Web
-Applications II</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Web
-Applications I
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Lab 2: Web Applications
-assigned</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Lecture 4: Web Applications
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Git Lab: Part I
-due</t>
-    </r>
   </si>
   <si>
     <t>Lab 3:
@@ -438,10 +372,79 @@
     </r>
   </si>
   <si>
-    <t>Lab 2: Web
-Application due
-7:00 am
+    <t>Web
+Applications II
+Web Applications Labs Review</t>
+  </si>
+  <si>
+    <t>Lab 2a: Web
+Applications
+due 7:00 am
 (Marmoset)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Lecture 4: Web Applications
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Git Lab: Part I
+due
+(in class)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Web
+Applications I
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Lab 2a: Web Applications
+(assigned)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Lecture 2:
+HTML &amp; CSS
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Lab 1: HTML &amp; CSS (assigned)</t>
+    </r>
+  </si>
+  <si>
+    <t>A06: Domain Analysis due
+(Google Doc)</t>
+  </si>
+  <si>
+    <t>CS320: SW Engineering - Spring 2020 Schedule
+(as of 1-15-2020, subject to change)</t>
   </si>
 </sst>
 </file>
@@ -1434,32 +1437,11 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -1467,6 +1449,42 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1474,21 +1492,6 @@
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1797,40 +1800,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" style="2" customWidth="1"/>
-    <col min="2" max="2" width="5" style="3" customWidth="1"/>
+    <col min="2" max="2" width="4.28515625" style="3" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" style="3" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" style="2" customWidth="1"/>
     <col min="5" max="5" width="13.140625" style="4" customWidth="1"/>
     <col min="6" max="6" width="13.42578125" style="2" customWidth="1"/>
     <col min="7" max="7" width="12.42578125" style="4" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" style="2" customWidth="1"/>
     <col min="9" max="9" width="13" style="3" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="57.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="115" t="s">
-        <v>59</v>
-      </c>
-      <c r="B1" s="116"/>
-      <c r="C1" s="116"/>
-      <c r="D1" s="116"/>
-      <c r="E1" s="116"/>
-      <c r="F1" s="116"/>
-      <c r="G1" s="116"/>
-      <c r="H1" s="116"/>
-      <c r="I1" s="117"/>
+      <c r="A1" s="126" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="127"/>
+      <c r="C1" s="127"/>
+      <c r="D1" s="127"/>
+      <c r="E1" s="127"/>
+      <c r="F1" s="127"/>
+      <c r="G1" s="127"/>
+      <c r="H1" s="127"/>
+      <c r="I1" s="128"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
@@ -1856,10 +1859,10 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="121">
+      <c r="A3" s="122">
         <v>16</v>
       </c>
-      <c r="B3" s="124" t="s">
+      <c r="B3" s="117" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="49">
@@ -1892,7 +1895,7 @@
     </row>
     <row r="4" spans="1:9" ht="70.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="120"/>
-      <c r="B4" s="125"/>
+      <c r="B4" s="118"/>
       <c r="C4" s="47" t="s">
         <v>8</v>
       </c>
@@ -1907,7 +1910,7 @@
       </c>
       <c r="G4" s="8"/>
       <c r="H4" s="80" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
       <c r="I4" s="84"/>
     </row>
@@ -1915,7 +1918,7 @@
       <c r="A5" s="120">
         <v>15</v>
       </c>
-      <c r="B5" s="125"/>
+      <c r="B5" s="118"/>
       <c r="C5" s="10">
         <f>I3 + 1</f>
         <v>26</v>
@@ -1945,31 +1948,31 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="90.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="122"/>
-      <c r="B6" s="125"/>
+      <c r="A6" s="123"/>
+      <c r="B6" s="118"/>
       <c r="C6" s="79" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D6" s="80" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="E6" s="81"/>
       <c r="F6" s="112" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="G6" s="8"/>
       <c r="H6" s="108" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="I6" s="111" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="121">
+      <c r="A7" s="122">
         <v>14</v>
       </c>
-      <c r="B7" s="126" t="s">
+      <c r="B7" s="131" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="82">
@@ -2002,29 +2005,29 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="123"/>
-      <c r="B8" s="127"/>
+      <c r="A8" s="121"/>
+      <c r="B8" s="132"/>
       <c r="C8" s="46" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E8" s="27"/>
       <c r="F8" s="27" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="G8" s="78"/>
       <c r="H8" s="72" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I8" s="42"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="119">
+      <c r="A9" s="130">
         <v>13</v>
       </c>
-      <c r="B9" s="127"/>
+      <c r="B9" s="132"/>
       <c r="C9" s="18">
         <f>I7 + 1</f>
         <v>9</v>
@@ -2056,20 +2059,20 @@
     </row>
     <row r="10" spans="1:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="120"/>
-      <c r="B10" s="127"/>
+      <c r="B10" s="132"/>
       <c r="C10" s="46" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D10" s="72" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E10" s="15"/>
       <c r="F10" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G10" s="15"/>
       <c r="H10" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I10" s="17"/>
     </row>
@@ -2077,7 +2080,7 @@
       <c r="A11" s="120">
         <v>12</v>
       </c>
-      <c r="B11" s="127"/>
+      <c r="B11" s="132"/>
       <c r="C11" s="21">
         <f>I9 + 1</f>
         <v>16</v>
@@ -2109,18 +2112,18 @@
     </row>
     <row r="12" spans="1:9" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="120"/>
-      <c r="B12" s="127"/>
+      <c r="B12" s="132"/>
       <c r="C12" s="43"/>
       <c r="D12" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E12" s="15"/>
       <c r="F12" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G12" s="15"/>
       <c r="H12" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I12" s="85"/>
     </row>
@@ -2128,7 +2131,7 @@
       <c r="A13" s="120">
         <v>11</v>
       </c>
-      <c r="B13" s="127"/>
+      <c r="B13" s="132"/>
       <c r="C13" s="21">
         <f>I11 + 1</f>
         <v>23</v>
@@ -2159,29 +2162,29 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="97.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="123"/>
-      <c r="B14" s="127"/>
+      <c r="A14" s="121"/>
+      <c r="B14" s="132"/>
       <c r="C14" s="43"/>
       <c r="D14" s="105" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E14" s="87"/>
       <c r="F14" s="40" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G14" s="103"/>
       <c r="H14" s="109" t="s">
         <v>17</v>
       </c>
       <c r="I14" s="57" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="121">
+      <c r="A15" s="122">
         <v>10</v>
       </c>
-      <c r="B15" s="126" t="s">
+      <c r="B15" s="131" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="49">
@@ -2212,9 +2215,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="122"/>
-      <c r="B16" s="128"/>
+    <row r="16" spans="1:9" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="123"/>
+      <c r="B16" s="133"/>
       <c r="C16" s="54" t="str">
         <f>I14</f>
         <v>WINTER BREAK</v>
@@ -2240,7 +2243,7 @@
         <v>WINTER BREAK</v>
       </c>
       <c r="I16" s="113" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="35" customFormat="1" ht="21.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -2259,7 +2262,7 @@
       <c r="B18" s="31"/>
       <c r="D18" s="34"/>
       <c r="E18" s="70" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F18" s="34"/>
       <c r="G18" s="34"/>
@@ -2271,7 +2274,7 @@
       <c r="B19" s="36"/>
       <c r="D19" s="30"/>
       <c r="E19" s="64" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F19" s="30"/>
       <c r="G19" s="30"/>
@@ -2283,7 +2286,7 @@
       <c r="B20" s="31"/>
       <c r="D20" s="34"/>
       <c r="E20" s="65" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F20" s="34"/>
       <c r="G20" s="34"/>
@@ -2295,7 +2298,7 @@
       <c r="B21" s="31"/>
       <c r="D21" s="34"/>
       <c r="E21" s="66" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F21" s="34"/>
       <c r="G21" s="34"/>
@@ -2307,7 +2310,7 @@
       <c r="B22" s="31"/>
       <c r="D22" s="34"/>
       <c r="E22" s="67" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F22" s="34"/>
       <c r="G22" s="34"/>
@@ -2320,7 +2323,7 @@
       <c r="C23" s="62"/>
       <c r="D23" s="34"/>
       <c r="E23" s="68" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F23" s="34"/>
       <c r="G23" s="34"/>
@@ -2350,19 +2353,19 @@
       <c r="I25" s="30"/>
     </row>
     <row r="26" spans="1:9" s="32" customFormat="1" ht="57.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="115" t="str">
+      <c r="A26" s="126" t="str">
         <f>A1</f>
         <v>CS320: SW Engineering - Spring 2020 Schedule
-(as of 1-14-2020, subject to change)</v>
-      </c>
-      <c r="B26" s="116"/>
-      <c r="C26" s="116"/>
-      <c r="D26" s="116"/>
-      <c r="E26" s="116"/>
-      <c r="F26" s="116"/>
-      <c r="G26" s="116"/>
-      <c r="H26" s="116"/>
-      <c r="I26" s="117"/>
+(as of 1-15-2020, subject to change)</v>
+      </c>
+      <c r="B26" s="127"/>
+      <c r="C26" s="127"/>
+      <c r="D26" s="127"/>
+      <c r="E26" s="127"/>
+      <c r="F26" s="127"/>
+      <c r="G26" s="127"/>
+      <c r="H26" s="127"/>
+      <c r="I26" s="128"/>
     </row>
     <row r="27" spans="1:9" s="2" customFormat="1" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="str">
@@ -2400,7 +2403,7 @@
       </c>
     </row>
     <row r="28" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="118">
+      <c r="A28" s="129">
         <v>10</v>
       </c>
       <c r="B28" s="73"/>
@@ -2433,9 +2436,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="119"/>
-      <c r="B29" s="125" t="s">
+    <row r="29" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="130"/>
+      <c r="B29" s="118" t="s">
         <v>13</v>
       </c>
       <c r="C29" s="47" t="str">
@@ -2464,14 +2467,15 @@
       </c>
       <c r="I29" s="45" t="str">
         <f t="shared" si="4"/>
-        <v>A06: Domain Analysis due</v>
+        <v>A06: Domain Analysis due
+(Google Doc)</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="119">
+      <c r="A30" s="130">
         <v>9</v>
       </c>
-      <c r="B30" s="125"/>
+      <c r="B30" s="118"/>
       <c r="C30" s="90">
         <f>I15 + 1</f>
         <v>8</v>
@@ -2503,21 +2507,21 @@
     </row>
     <row r="31" spans="1:9" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="120"/>
-      <c r="B31" s="125"/>
+      <c r="B31" s="118"/>
       <c r="C31" s="91" t="str">
         <f>H29</f>
         <v>WINTER BREAK</v>
       </c>
       <c r="D31" s="37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E31" s="7"/>
       <c r="F31" s="24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G31" s="7"/>
       <c r="H31" s="105" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I31" s="71"/>
     </row>
@@ -2525,7 +2529,7 @@
       <c r="A32" s="120">
         <v>8</v>
       </c>
-      <c r="B32" s="125"/>
+      <c r="B32" s="118"/>
       <c r="C32" s="25">
         <f>I30 + 1</f>
         <v>15</v>
@@ -2557,22 +2561,22 @@
     </row>
     <row r="33" spans="1:9" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="120"/>
-      <c r="B33" s="125"/>
+      <c r="B33" s="118"/>
       <c r="C33" s="96" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D33" s="28" t="s">
         <v>16</v>
       </c>
       <c r="E33" s="96" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G33" s="7"/>
       <c r="H33" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I33" s="71"/>
     </row>
@@ -2580,7 +2584,7 @@
       <c r="A34" s="120">
         <v>7</v>
       </c>
-      <c r="B34" s="125"/>
+      <c r="B34" s="118"/>
       <c r="C34" s="10">
         <f>I32 + 1</f>
         <v>22</v>
@@ -2612,19 +2616,19 @@
     </row>
     <row r="35" spans="1:9" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="120"/>
-      <c r="B35" s="125"/>
+      <c r="B35" s="118"/>
       <c r="C35" s="10"/>
       <c r="D35" s="98" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E35" s="96" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F35" s="7" t="s">
         <v>18</v>
       </c>
       <c r="G35" s="69" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H35" s="24" t="s">
         <v>19</v>
@@ -2665,17 +2669,17 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="69.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="122"/>
+      <c r="A37" s="123"/>
       <c r="B37" s="75"/>
       <c r="C37" s="110"/>
       <c r="D37" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E37" s="113" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F37" s="72" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="G37" s="41"/>
       <c r="H37" s="94" t="s">
@@ -2684,10 +2688,10 @@
       <c r="I37" s="42"/>
     </row>
     <row r="38" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="121">
+      <c r="A38" s="122">
         <v>5</v>
       </c>
-      <c r="B38" s="129" t="s">
+      <c r="B38" s="115" t="s">
         <v>14</v>
       </c>
       <c r="C38" s="43">
@@ -2721,10 +2725,10 @@
     </row>
     <row r="39" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="120"/>
-      <c r="B39" s="130"/>
+      <c r="B39" s="116"/>
       <c r="C39" s="43"/>
       <c r="D39" s="72" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E39" s="106"/>
       <c r="F39" s="27" t="s">
@@ -2744,7 +2748,7 @@
       <c r="A40" s="120">
         <v>4</v>
       </c>
-      <c r="B40" s="130"/>
+      <c r="B40" s="116"/>
       <c r="C40" s="48">
         <f>I38 + 1</f>
         <v>12</v>
@@ -2774,9 +2778,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="120"/>
-      <c r="B41" s="130"/>
+      <c r="B41" s="116"/>
       <c r="C41" s="47" t="s">
         <v>6</v>
       </c>
@@ -2797,7 +2801,7 @@
       <c r="A42" s="120">
         <v>3</v>
       </c>
-      <c r="B42" s="130"/>
+      <c r="B42" s="116"/>
       <c r="C42" s="43">
         <f>I40 + 1</f>
         <v>19</v>
@@ -2829,14 +2833,14 @@
     </row>
     <row r="43" spans="1:9" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="120"/>
-      <c r="B43" s="130"/>
+      <c r="B43" s="116"/>
       <c r="C43" s="43"/>
       <c r="D43" s="92" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E43" s="15"/>
       <c r="F43" s="95" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G43" s="87"/>
       <c r="H43" s="95" t="s">
@@ -2848,7 +2852,7 @@
       <c r="A44" s="120">
         <v>2</v>
       </c>
-      <c r="B44" s="130"/>
+      <c r="B44" s="116"/>
       <c r="C44" s="21">
         <f>I42 + 1</f>
         <v>26</v>
@@ -2877,9 +2881,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="122"/>
-      <c r="B45" s="130"/>
+    <row r="45" spans="1:9" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="123"/>
+      <c r="B45" s="116"/>
       <c r="C45" s="97"/>
       <c r="D45" s="109" t="s">
         <v>7</v>
@@ -2895,10 +2899,10 @@
       <c r="I45" s="9"/>
     </row>
     <row r="46" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="121">
+      <c r="A46" s="122">
         <v>1</v>
       </c>
-      <c r="B46" s="124" t="s">
+      <c r="B46" s="117" t="s">
         <v>5</v>
       </c>
       <c r="C46" s="38">
@@ -2930,9 +2934,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="120"/>
-      <c r="B47" s="125"/>
+      <c r="B47" s="118"/>
       <c r="C47" s="39"/>
       <c r="D47" s="7" t="s">
         <v>7</v>
@@ -2943,17 +2947,17 @@
       </c>
       <c r="G47" s="44"/>
       <c r="H47" s="114" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="I47" s="45" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="132" t="s">
-        <v>60</v>
-      </c>
-      <c r="B48" s="125"/>
+      <c r="A48" s="124" t="s">
+        <v>57</v>
+      </c>
+      <c r="B48" s="118"/>
       <c r="C48" s="25">
         <f>I46 + 1</f>
         <v>10</v>
@@ -2984,17 +2988,17 @@
       </c>
     </row>
     <row r="49" spans="1:9" ht="144" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="133"/>
-      <c r="B49" s="131"/>
+      <c r="A49" s="125"/>
+      <c r="B49" s="119"/>
       <c r="C49" s="69" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D49" s="29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E49" s="26"/>
       <c r="F49" s="29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G49" s="26"/>
       <c r="H49" s="12"/>
@@ -3003,6 +3007,19 @@
     <row r="50" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="B7:B14"/>
+    <mergeCell ref="A26:I26"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B29:B35"/>
     <mergeCell ref="B38:B45"/>
     <mergeCell ref="B46:B49"/>
     <mergeCell ref="A13:A14"/>
@@ -3016,21 +3033,8 @@
     <mergeCell ref="A36:A37"/>
     <mergeCell ref="A38:A39"/>
     <mergeCell ref="A40:A41"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="B7:B14"/>
-    <mergeCell ref="A26:I26"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B29:B35"/>
   </mergeCells>
-  <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0" footer="0"/>
   <pageSetup paperSize="5" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
moved lab01 due date
</commit_message>
<xml_diff>
--- a/CS320-Spring2020Calendar.xlsx
+++ b/CS320-Spring2020Calendar.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\djhake2\cs320-spring2020\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="315" yWindow="-165" windowWidth="13305" windowHeight="13905"/>
   </bookViews>
@@ -11,7 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -219,11 +224,6 @@
 103: 3:00-5:00
 A08: Team Presentation and Demonstration
 (in class)</t>
-  </si>
-  <si>
-    <t>Lab 1: HTML &amp; CSS  due
-7:00 am
-(Marmoset)</t>
   </si>
   <si>
     <t>A01: Team Project Proposal due
@@ -443,8 +443,15 @@
 (Google Doc)</t>
   </si>
   <si>
+    <t>Lab 1: HTML &amp; CSS  due
+7:00 am
+MONDAY ---&gt;
+(1-27-20)
+(Marmoset)</t>
+  </si>
+  <si>
     <t>CS320: SW Engineering - Spring 2020 Schedule
-(as of 1-15-2020, subject to change)</t>
+(as of 1-24-2020, subject to change)</t>
   </si>
 </sst>
 </file>
@@ -1093,7 +1100,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1435,6 +1442,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1554,7 +1564,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1589,7 +1599,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1798,16 +1808,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:I50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7" style="2" customWidth="1"/>
-    <col min="2" max="2" width="4.28515625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="4.42578125" style="3" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" style="3" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" style="2" customWidth="1"/>
     <col min="5" max="5" width="13.140625" style="4" customWidth="1"/>
@@ -1819,20 +1832,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="57.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="126" t="s">
+      <c r="A1" s="127" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="127"/>
-      <c r="C1" s="127"/>
-      <c r="D1" s="127"/>
-      <c r="E1" s="127"/>
-      <c r="F1" s="127"/>
-      <c r="G1" s="127"/>
-      <c r="H1" s="127"/>
-      <c r="I1" s="128"/>
-    </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="B1" s="128"/>
+      <c r="C1" s="128"/>
+      <c r="D1" s="128"/>
+      <c r="E1" s="128"/>
+      <c r="F1" s="128"/>
+      <c r="G1" s="128"/>
+      <c r="H1" s="128"/>
+      <c r="I1" s="129"/>
+    </row>
+    <row r="2" spans="1:9" s="2" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="115" t="s">
         <v>31</v>
       </c>
       <c r="B2" s="1"/>
@@ -1859,10 +1872,10 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="122">
+      <c r="A3" s="123">
         <v>16</v>
       </c>
-      <c r="B3" s="117" t="s">
+      <c r="B3" s="118" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="49">
@@ -1894,8 +1907,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="70.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="120"/>
-      <c r="B4" s="118"/>
+      <c r="A4" s="121"/>
+      <c r="B4" s="119"/>
       <c r="C4" s="47" t="s">
         <v>8</v>
       </c>
@@ -1910,15 +1923,15 @@
       </c>
       <c r="G4" s="8"/>
       <c r="H4" s="80" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I4" s="84"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="120">
+      <c r="A5" s="121">
         <v>15</v>
       </c>
-      <c r="B5" s="118"/>
+      <c r="B5" s="119"/>
       <c r="C5" s="10">
         <f>I3 + 1</f>
         <v>26</v>
@@ -1948,31 +1961,31 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="90.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="123"/>
-      <c r="B6" s="118"/>
+      <c r="A6" s="124"/>
+      <c r="B6" s="119"/>
       <c r="C6" s="79" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="D6" s="80" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E6" s="81"/>
       <c r="F6" s="112" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G6" s="8"/>
       <c r="H6" s="108" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I6" s="111" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="122">
+      <c r="A7" s="123">
         <v>14</v>
       </c>
-      <c r="B7" s="131" t="s">
+      <c r="B7" s="132" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="82">
@@ -2005,17 +2018,17 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="121"/>
-      <c r="B8" s="132"/>
+      <c r="A8" s="122"/>
+      <c r="B8" s="133"/>
       <c r="C8" s="46" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E8" s="27"/>
       <c r="F8" s="27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G8" s="78"/>
       <c r="H8" s="72" t="s">
@@ -2024,10 +2037,10 @@
       <c r="I8" s="42"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="130">
+      <c r="A9" s="131">
         <v>13</v>
       </c>
-      <c r="B9" s="132"/>
+      <c r="B9" s="133"/>
       <c r="C9" s="18">
         <f>I7 + 1</f>
         <v>9</v>
@@ -2058,10 +2071,10 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="120"/>
-      <c r="B10" s="132"/>
+      <c r="A10" s="121"/>
+      <c r="B10" s="133"/>
       <c r="C10" s="46" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D10" s="72" t="s">
         <v>37</v>
@@ -2077,10 +2090,10 @@
       <c r="I10" s="17"/>
     </row>
     <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="120">
+      <c r="A11" s="121">
         <v>12</v>
       </c>
-      <c r="B11" s="132"/>
+      <c r="B11" s="133"/>
       <c r="C11" s="21">
         <f>I9 + 1</f>
         <v>16</v>
@@ -2111,8 +2124,8 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="120"/>
-      <c r="B12" s="132"/>
+      <c r="A12" s="121"/>
+      <c r="B12" s="133"/>
       <c r="C12" s="43"/>
       <c r="D12" s="37" t="s">
         <v>36</v>
@@ -2128,10 +2141,10 @@
       <c r="I12" s="85"/>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="120">
+      <c r="A13" s="121">
         <v>11</v>
       </c>
-      <c r="B13" s="132"/>
+      <c r="B13" s="133"/>
       <c r="C13" s="21">
         <f>I11 + 1</f>
         <v>23</v>
@@ -2162,11 +2175,11 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="97.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="121"/>
-      <c r="B14" s="132"/>
+      <c r="A14" s="122"/>
+      <c r="B14" s="133"/>
       <c r="C14" s="43"/>
       <c r="D14" s="105" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E14" s="87"/>
       <c r="F14" s="40" t="s">
@@ -2181,10 +2194,10 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="122">
+      <c r="A15" s="123">
         <v>10</v>
       </c>
-      <c r="B15" s="131" t="s">
+      <c r="B15" s="132" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="49">
@@ -2216,8 +2229,8 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="123"/>
-      <c r="B16" s="133"/>
+      <c r="A16" s="124"/>
+      <c r="B16" s="134"/>
       <c r="C16" s="54" t="str">
         <f>I14</f>
         <v>WINTER BREAK</v>
@@ -2243,7 +2256,7 @@
         <v>WINTER BREAK</v>
       </c>
       <c r="I16" s="113" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="35" customFormat="1" ht="21.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -2353,19 +2366,19 @@
       <c r="I25" s="30"/>
     </row>
     <row r="26" spans="1:9" s="32" customFormat="1" ht="57.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="126" t="str">
+      <c r="A26" s="127" t="str">
         <f>A1</f>
         <v>CS320: SW Engineering - Spring 2020 Schedule
-(as of 1-15-2020, subject to change)</v>
-      </c>
-      <c r="B26" s="127"/>
-      <c r="C26" s="127"/>
-      <c r="D26" s="127"/>
-      <c r="E26" s="127"/>
-      <c r="F26" s="127"/>
-      <c r="G26" s="127"/>
-      <c r="H26" s="127"/>
-      <c r="I26" s="128"/>
+(as of 1-24-2020, subject to change)</v>
+      </c>
+      <c r="B26" s="128"/>
+      <c r="C26" s="128"/>
+      <c r="D26" s="128"/>
+      <c r="E26" s="128"/>
+      <c r="F26" s="128"/>
+      <c r="G26" s="128"/>
+      <c r="H26" s="128"/>
+      <c r="I26" s="129"/>
     </row>
     <row r="27" spans="1:9" s="2" customFormat="1" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="str">
@@ -2403,7 +2416,7 @@
       </c>
     </row>
     <row r="28" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="129">
+      <c r="A28" s="130">
         <v>10</v>
       </c>
       <c r="B28" s="73"/>
@@ -2437,8 +2450,8 @@
       </c>
     </row>
     <row r="29" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="130"/>
-      <c r="B29" s="118" t="s">
+      <c r="A29" s="131"/>
+      <c r="B29" s="119" t="s">
         <v>13</v>
       </c>
       <c r="C29" s="47" t="str">
@@ -2472,10 +2485,10 @@
       </c>
     </row>
     <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="130">
+      <c r="A30" s="131">
         <v>9</v>
       </c>
-      <c r="B30" s="118"/>
+      <c r="B30" s="119"/>
       <c r="C30" s="90">
         <f>I15 + 1</f>
         <v>8</v>
@@ -2506,8 +2519,8 @@
       </c>
     </row>
     <row r="31" spans="1:9" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="120"/>
-      <c r="B31" s="118"/>
+      <c r="A31" s="121"/>
+      <c r="B31" s="119"/>
       <c r="C31" s="91" t="str">
         <f>H29</f>
         <v>WINTER BREAK</v>
@@ -2521,15 +2534,15 @@
       </c>
       <c r="G31" s="7"/>
       <c r="H31" s="105" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I31" s="71"/>
     </row>
     <row r="32" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="120">
+      <c r="A32" s="121">
         <v>8</v>
       </c>
-      <c r="B32" s="118"/>
+      <c r="B32" s="119"/>
       <c r="C32" s="25">
         <f>I30 + 1</f>
         <v>15</v>
@@ -2560,16 +2573,16 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="120"/>
-      <c r="B33" s="118"/>
+      <c r="A33" s="121"/>
+      <c r="B33" s="119"/>
       <c r="C33" s="96" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D33" s="28" t="s">
         <v>16</v>
       </c>
       <c r="E33" s="96" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F33" s="7" t="s">
         <v>22</v>
@@ -2581,10 +2594,10 @@
       <c r="I33" s="71"/>
     </row>
     <row r="34" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="120">
+      <c r="A34" s="121">
         <v>7</v>
       </c>
-      <c r="B34" s="118"/>
+      <c r="B34" s="119"/>
       <c r="C34" s="10">
         <f>I32 + 1</f>
         <v>22</v>
@@ -2615,20 +2628,20 @@
       </c>
     </row>
     <row r="35" spans="1:9" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="120"/>
-      <c r="B35" s="118"/>
+      <c r="A35" s="121"/>
+      <c r="B35" s="119"/>
       <c r="C35" s="10"/>
       <c r="D35" s="98" t="s">
         <v>43</v>
       </c>
       <c r="E35" s="96" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F35" s="7" t="s">
         <v>18</v>
       </c>
       <c r="G35" s="69" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H35" s="24" t="s">
         <v>19</v>
@@ -2636,7 +2649,7 @@
       <c r="I35" s="42"/>
     </row>
     <row r="36" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="120">
+      <c r="A36" s="121">
         <v>6</v>
       </c>
       <c r="B36" s="74"/>
@@ -2669,17 +2682,17 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="69.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="123"/>
+      <c r="A37" s="124"/>
       <c r="B37" s="75"/>
       <c r="C37" s="110"/>
       <c r="D37" s="29" t="s">
         <v>33</v>
       </c>
       <c r="E37" s="113" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F37" s="72" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G37" s="41"/>
       <c r="H37" s="94" t="s">
@@ -2688,10 +2701,10 @@
       <c r="I37" s="42"/>
     </row>
     <row r="38" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="122">
+      <c r="A38" s="123">
         <v>5</v>
       </c>
-      <c r="B38" s="115" t="s">
+      <c r="B38" s="116" t="s">
         <v>14</v>
       </c>
       <c r="C38" s="43">
@@ -2724,11 +2737,11 @@
       </c>
     </row>
     <row r="39" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="120"/>
-      <c r="B39" s="116"/>
+      <c r="A39" s="121"/>
+      <c r="B39" s="117"/>
       <c r="C39" s="43"/>
       <c r="D39" s="72" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E39" s="106"/>
       <c r="F39" s="27" t="s">
@@ -2745,10 +2758,10 @@
       </c>
     </row>
     <row r="40" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="120">
+      <c r="A40" s="121">
         <v>4</v>
       </c>
-      <c r="B40" s="116"/>
+      <c r="B40" s="117"/>
       <c r="C40" s="48">
         <f>I38 + 1</f>
         <v>12</v>
@@ -2779,8 +2792,8 @@
       </c>
     </row>
     <row r="41" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="120"/>
-      <c r="B41" s="116"/>
+      <c r="A41" s="121"/>
+      <c r="B41" s="117"/>
       <c r="C41" s="47" t="s">
         <v>6</v>
       </c>
@@ -2798,10 +2811,10 @@
       <c r="I41" s="42"/>
     </row>
     <row r="42" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="120">
+      <c r="A42" s="121">
         <v>3</v>
       </c>
-      <c r="B42" s="116"/>
+      <c r="B42" s="117"/>
       <c r="C42" s="43">
         <f>I40 + 1</f>
         <v>19</v>
@@ -2832,15 +2845,15 @@
       </c>
     </row>
     <row r="43" spans="1:9" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="120"/>
-      <c r="B43" s="116"/>
+      <c r="A43" s="121"/>
+      <c r="B43" s="117"/>
       <c r="C43" s="43"/>
       <c r="D43" s="92" t="s">
         <v>35</v>
       </c>
       <c r="E43" s="15"/>
       <c r="F43" s="95" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G43" s="87"/>
       <c r="H43" s="95" t="s">
@@ -2849,10 +2862,10 @@
       <c r="I43" s="85"/>
     </row>
     <row r="44" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="120">
+      <c r="A44" s="121">
         <v>2</v>
       </c>
-      <c r="B44" s="116"/>
+      <c r="B44" s="117"/>
       <c r="C44" s="21">
         <f>I42 + 1</f>
         <v>26</v>
@@ -2882,8 +2895,8 @@
       </c>
     </row>
     <row r="45" spans="1:9" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="123"/>
-      <c r="B45" s="116"/>
+      <c r="A45" s="124"/>
+      <c r="B45" s="117"/>
       <c r="C45" s="97"/>
       <c r="D45" s="109" t="s">
         <v>7</v>
@@ -2899,10 +2912,10 @@
       <c r="I45" s="9"/>
     </row>
     <row r="46" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="122">
+      <c r="A46" s="123">
         <v>1</v>
       </c>
-      <c r="B46" s="117" t="s">
+      <c r="B46" s="118" t="s">
         <v>5</v>
       </c>
       <c r="C46" s="38">
@@ -2935,8 +2948,8 @@
       </c>
     </row>
     <row r="47" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="120"/>
-      <c r="B47" s="118"/>
+      <c r="A47" s="121"/>
+      <c r="B47" s="119"/>
       <c r="C47" s="39"/>
       <c r="D47" s="7" t="s">
         <v>7</v>
@@ -2947,17 +2960,17 @@
       </c>
       <c r="G47" s="44"/>
       <c r="H47" s="114" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I47" s="45" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="124" t="s">
-        <v>57</v>
-      </c>
-      <c r="B48" s="118"/>
+      <c r="A48" s="125" t="s">
+        <v>56</v>
+      </c>
+      <c r="B48" s="119"/>
       <c r="C48" s="25">
         <f>I46 + 1</f>
         <v>10</v>
@@ -2988,10 +3001,10 @@
       </c>
     </row>
     <row r="49" spans="1:9" ht="144" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="125"/>
-      <c r="B49" s="119"/>
+      <c r="A49" s="126"/>
+      <c r="B49" s="120"/>
       <c r="C49" s="69" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D49" s="29" t="s">
         <v>45</v>
@@ -3034,8 +3047,8 @@
     <mergeCell ref="A38:A39"/>
     <mergeCell ref="A40:A41"/>
   </mergeCells>
-  <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0" footer="0"/>
-  <pageSetup paperSize="5" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="5" scale="99" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
updated news and lab05 due date
</commit_message>
<xml_diff>
--- a/CS320-Spring2020Calendar.xlsx
+++ b/CS320-Spring2020Calendar.xlsx
@@ -424,10 +424,6 @@
 (Marmoset)</t>
   </si>
   <si>
-    <t>CS320: SW Engineering - Spring 2020 Schedule
-(as of 2-2-2020, subject to change)</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Web
 Applications II
@@ -470,6 +466,10 @@
 due 7:00 am
 MONDAY ---&gt;
 (Marmoset)</t>
+  </si>
+  <si>
+    <t>CS320: SW Engineering - Spring 2020 Schedule
+(as of 3-5-2020, subject to change)</t>
   </si>
 </sst>
 </file>
@@ -1462,32 +1462,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -1495,6 +1477,42 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1503,24 +1521,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1831,8 +1831,8 @@
   </sheetPr>
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1850,17 +1850,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="57.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="115" t="s">
-        <v>66</v>
-      </c>
-      <c r="B1" s="116"/>
-      <c r="C1" s="116"/>
-      <c r="D1" s="116"/>
-      <c r="E1" s="116"/>
-      <c r="F1" s="116"/>
-      <c r="G1" s="116"/>
-      <c r="H1" s="116"/>
-      <c r="I1" s="117"/>
+      <c r="A1" s="127" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="128"/>
+      <c r="C1" s="128"/>
+      <c r="D1" s="128"/>
+      <c r="E1" s="128"/>
+      <c r="F1" s="128"/>
+      <c r="G1" s="128"/>
+      <c r="H1" s="128"/>
+      <c r="I1" s="129"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="114" t="s">
@@ -1890,10 +1890,10 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="121">
+      <c r="A3" s="123">
         <v>16</v>
       </c>
-      <c r="B3" s="124" t="s">
+      <c r="B3" s="118" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="49">
@@ -1925,8 +1925,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="70.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="120"/>
-      <c r="B4" s="125"/>
+      <c r="A4" s="121"/>
+      <c r="B4" s="119"/>
       <c r="C4" s="47" t="s">
         <v>8</v>
       </c>
@@ -1946,10 +1946,10 @@
       <c r="I4" s="84"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="120">
+      <c r="A5" s="121">
         <v>15</v>
       </c>
-      <c r="B5" s="125"/>
+      <c r="B5" s="119"/>
       <c r="C5" s="10">
         <f>I3 + 1</f>
         <v>26</v>
@@ -1979,8 +1979,8 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="90.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="122"/>
-      <c r="B6" s="125"/>
+      <c r="A6" s="124"/>
+      <c r="B6" s="119"/>
       <c r="C6" s="79" t="s">
         <v>65</v>
       </c>
@@ -1995,13 +1995,13 @@
       <c r="H6" s="108" t="s">
         <v>62</v>
       </c>
-      <c r="I6" s="134"/>
+      <c r="I6" s="115"/>
     </row>
     <row r="7" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="121">
+      <c r="A7" s="123">
         <v>14</v>
       </c>
-      <c r="B7" s="126" t="s">
+      <c r="B7" s="132" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="82">
@@ -2034,13 +2034,13 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="123"/>
-      <c r="B8" s="127"/>
+      <c r="A8" s="122"/>
+      <c r="B8" s="133"/>
       <c r="C8" s="46" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D8" s="105" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E8" s="27"/>
       <c r="F8" s="27" t="s">
@@ -2053,10 +2053,10 @@
       <c r="I8" s="42"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="119">
+      <c r="A9" s="131">
         <v>13</v>
       </c>
-      <c r="B9" s="127"/>
+      <c r="B9" s="133"/>
       <c r="C9" s="18">
         <f>I7 + 1</f>
         <v>9</v>
@@ -2087,10 +2087,10 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="120"/>
-      <c r="B10" s="127"/>
+      <c r="A10" s="121"/>
+      <c r="B10" s="133"/>
       <c r="C10" s="46" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D10" s="72" t="s">
         <v>37</v>
@@ -2106,10 +2106,10 @@
       <c r="I10" s="17"/>
     </row>
     <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="120">
+      <c r="A11" s="121">
         <v>12</v>
       </c>
-      <c r="B11" s="127"/>
+      <c r="B11" s="133"/>
       <c r="C11" s="21">
         <f>I9 + 1</f>
         <v>16</v>
@@ -2140,8 +2140,8 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="120"/>
-      <c r="B12" s="127"/>
+      <c r="A12" s="121"/>
+      <c r="B12" s="133"/>
       <c r="C12" s="43"/>
       <c r="D12" s="37" t="s">
         <v>36</v>
@@ -2157,10 +2157,10 @@
       <c r="I12" s="85"/>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="120">
+      <c r="A13" s="121">
         <v>11</v>
       </c>
-      <c r="B13" s="127"/>
+      <c r="B13" s="133"/>
       <c r="C13" s="21">
         <f>I11 + 1</f>
         <v>23</v>
@@ -2191,8 +2191,8 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="97.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="123"/>
-      <c r="B14" s="127"/>
+      <c r="A14" s="122"/>
+      <c r="B14" s="133"/>
       <c r="C14" s="43"/>
       <c r="D14" s="105" t="s">
         <v>56</v>
@@ -2210,10 +2210,10 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="121">
+      <c r="A15" s="123">
         <v>10</v>
       </c>
-      <c r="B15" s="126" t="s">
+      <c r="B15" s="132" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="49">
@@ -2245,8 +2245,8 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="122"/>
-      <c r="B16" s="128"/>
+      <c r="A16" s="124"/>
+      <c r="B16" s="134"/>
       <c r="C16" s="54" t="str">
         <f>I14</f>
         <v>WINTER BREAK</v>
@@ -2382,19 +2382,19 @@
       <c r="I25" s="30"/>
     </row>
     <row r="26" spans="1:9" s="32" customFormat="1" ht="57.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="115" t="str">
+      <c r="A26" s="127" t="str">
         <f>A1</f>
         <v>CS320: SW Engineering - Spring 2020 Schedule
-(as of 2-2-2020, subject to change)</v>
-      </c>
-      <c r="B26" s="116"/>
-      <c r="C26" s="116"/>
-      <c r="D26" s="116"/>
-      <c r="E26" s="116"/>
-      <c r="F26" s="116"/>
-      <c r="G26" s="116"/>
-      <c r="H26" s="116"/>
-      <c r="I26" s="117"/>
+(as of 3-5-2020, subject to change)</v>
+      </c>
+      <c r="B26" s="128"/>
+      <c r="C26" s="128"/>
+      <c r="D26" s="128"/>
+      <c r="E26" s="128"/>
+      <c r="F26" s="128"/>
+      <c r="G26" s="128"/>
+      <c r="H26" s="128"/>
+      <c r="I26" s="129"/>
     </row>
     <row r="27" spans="1:9" s="2" customFormat="1" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="str">
@@ -2432,7 +2432,7 @@
       </c>
     </row>
     <row r="28" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="118">
+      <c r="A28" s="130">
         <v>10</v>
       </c>
       <c r="B28" s="73"/>
@@ -2466,8 +2466,8 @@
       </c>
     </row>
     <row r="29" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="119"/>
-      <c r="B29" s="125" t="s">
+      <c r="A29" s="131"/>
+      <c r="B29" s="119" t="s">
         <v>13</v>
       </c>
       <c r="C29" s="47" t="str">
@@ -2501,10 +2501,10 @@
       </c>
     </row>
     <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="119">
+      <c r="A30" s="131">
         <v>9</v>
       </c>
-      <c r="B30" s="125"/>
+      <c r="B30" s="119"/>
       <c r="C30" s="90">
         <f>I15 + 1</f>
         <v>8</v>
@@ -2535,8 +2535,8 @@
       </c>
     </row>
     <row r="31" spans="1:9" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="120"/>
-      <c r="B31" s="125"/>
+      <c r="A31" s="121"/>
+      <c r="B31" s="119"/>
       <c r="C31" s="91" t="str">
         <f>H29</f>
         <v>WINTER BREAK</v>
@@ -2555,10 +2555,10 @@
       <c r="I31" s="71"/>
     </row>
     <row r="32" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="120">
+      <c r="A32" s="121">
         <v>8</v>
       </c>
-      <c r="B32" s="125"/>
+      <c r="B32" s="119"/>
       <c r="C32" s="25">
         <f>I30 + 1</f>
         <v>15</v>
@@ -2589,11 +2589,9 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="120"/>
-      <c r="B33" s="125"/>
-      <c r="C33" s="96" t="s">
-        <v>46</v>
-      </c>
+      <c r="A33" s="121"/>
+      <c r="B33" s="119"/>
+      <c r="C33" s="10"/>
       <c r="D33" s="28" t="s">
         <v>16</v>
       </c>
@@ -2603,17 +2601,19 @@
       <c r="F33" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G33" s="7"/>
+      <c r="G33" s="96" t="s">
+        <v>46</v>
+      </c>
       <c r="H33" s="7" t="s">
         <v>34</v>
       </c>
       <c r="I33" s="71"/>
     </row>
     <row r="34" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="120">
+      <c r="A34" s="121">
         <v>7</v>
       </c>
-      <c r="B34" s="125"/>
+      <c r="B34" s="119"/>
       <c r="C34" s="10">
         <f>I32 + 1</f>
         <v>22</v>
@@ -2644,8 +2644,8 @@
       </c>
     </row>
     <row r="35" spans="1:9" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="120"/>
-      <c r="B35" s="125"/>
+      <c r="A35" s="121"/>
+      <c r="B35" s="119"/>
       <c r="C35" s="10"/>
       <c r="D35" s="98" t="s">
         <v>43</v>
@@ -2665,7 +2665,7 @@
       <c r="I35" s="42"/>
     </row>
     <row r="36" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="120">
+      <c r="A36" s="121">
         <v>6</v>
       </c>
       <c r="B36" s="74"/>
@@ -2698,7 +2698,7 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="69.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="122"/>
+      <c r="A37" s="124"/>
       <c r="B37" s="75"/>
       <c r="C37" s="110"/>
       <c r="D37" s="29" t="s">
@@ -2717,10 +2717,10 @@
       <c r="I37" s="42"/>
     </row>
     <row r="38" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="121">
+      <c r="A38" s="123">
         <v>5</v>
       </c>
-      <c r="B38" s="129" t="s">
+      <c r="B38" s="116" t="s">
         <v>14</v>
       </c>
       <c r="C38" s="43">
@@ -2753,8 +2753,8 @@
       </c>
     </row>
     <row r="39" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="120"/>
-      <c r="B39" s="130"/>
+      <c r="A39" s="121"/>
+      <c r="B39" s="117"/>
       <c r="C39" s="43"/>
       <c r="D39" s="72" t="s">
         <v>59</v>
@@ -2774,10 +2774,10 @@
       </c>
     </row>
     <row r="40" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="120">
+      <c r="A40" s="121">
         <v>4</v>
       </c>
-      <c r="B40" s="130"/>
+      <c r="B40" s="117"/>
       <c r="C40" s="48">
         <f>I38 + 1</f>
         <v>12</v>
@@ -2808,8 +2808,8 @@
       </c>
     </row>
     <row r="41" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="120"/>
-      <c r="B41" s="130"/>
+      <c r="A41" s="121"/>
+      <c r="B41" s="117"/>
       <c r="C41" s="47" t="s">
         <v>6</v>
       </c>
@@ -2827,10 +2827,10 @@
       <c r="I41" s="42"/>
     </row>
     <row r="42" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="120">
+      <c r="A42" s="121">
         <v>3</v>
       </c>
-      <c r="B42" s="130"/>
+      <c r="B42" s="117"/>
       <c r="C42" s="43">
         <f>I40 + 1</f>
         <v>19</v>
@@ -2861,8 +2861,8 @@
       </c>
     </row>
     <row r="43" spans="1:9" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="120"/>
-      <c r="B43" s="130"/>
+      <c r="A43" s="121"/>
+      <c r="B43" s="117"/>
       <c r="C43" s="43"/>
       <c r="D43" s="92" t="s">
         <v>35</v>
@@ -2878,10 +2878,10 @@
       <c r="I43" s="85"/>
     </row>
     <row r="44" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="120">
+      <c r="A44" s="121">
         <v>2</v>
       </c>
-      <c r="B44" s="130"/>
+      <c r="B44" s="117"/>
       <c r="C44" s="21">
         <f>I42 + 1</f>
         <v>26</v>
@@ -2911,8 +2911,8 @@
       </c>
     </row>
     <row r="45" spans="1:9" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="122"/>
-      <c r="B45" s="130"/>
+      <c r="A45" s="124"/>
+      <c r="B45" s="117"/>
       <c r="C45" s="97"/>
       <c r="D45" s="109" t="s">
         <v>7</v>
@@ -2928,10 +2928,10 @@
       <c r="I45" s="9"/>
     </row>
     <row r="46" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="121">
+      <c r="A46" s="123">
         <v>1</v>
       </c>
-      <c r="B46" s="124" t="s">
+      <c r="B46" s="118" t="s">
         <v>5</v>
       </c>
       <c r="C46" s="38">
@@ -2964,8 +2964,8 @@
       </c>
     </row>
     <row r="47" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="120"/>
-      <c r="B47" s="125"/>
+      <c r="A47" s="121"/>
+      <c r="B47" s="119"/>
       <c r="C47" s="39"/>
       <c r="D47" s="7" t="s">
         <v>7</v>
@@ -2983,10 +2983,10 @@
       </c>
     </row>
     <row r="48" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="132" t="s">
+      <c r="A48" s="125" t="s">
         <v>54</v>
       </c>
-      <c r="B48" s="125"/>
+      <c r="B48" s="119"/>
       <c r="C48" s="25">
         <f>I46 + 1</f>
         <v>10</v>
@@ -3017,8 +3017,8 @@
       </c>
     </row>
     <row r="49" spans="1:9" ht="144" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="133"/>
-      <c r="B49" s="131"/>
+      <c r="A49" s="126"/>
+      <c r="B49" s="120"/>
       <c r="C49" s="69" t="s">
         <v>51</v>
       </c>
@@ -3036,6 +3036,19 @@
     <row r="50" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="B7:B14"/>
+    <mergeCell ref="A26:I26"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B29:B35"/>
     <mergeCell ref="B38:B45"/>
     <mergeCell ref="B46:B49"/>
     <mergeCell ref="A13:A14"/>
@@ -3049,19 +3062,6 @@
     <mergeCell ref="A36:A37"/>
     <mergeCell ref="A38:A39"/>
     <mergeCell ref="A40:A41"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="B7:B14"/>
-    <mergeCell ref="A26:I26"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B29:B35"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" scale="99" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated schedule due to school closure and remote teaching)
</commit_message>
<xml_diff>
--- a/CS320-Spring2020Calendar.xlsx
+++ b/CS320-Spring2020Calendar.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="71">
   <si>
     <t>Monday</t>
   </si>
@@ -65,23 +65,8 @@
     <t>April</t>
   </si>
   <si>
-    <t>Mid-Term
-Exam
-(in-class)</t>
-  </si>
-  <si>
-    <t>A03: Team MS1
-Minimal Working System</t>
-  </si>
-  <si>
     <t>Lecture 11: OO Design, OCP, LSP
 Design Principles and Design Patterns</t>
-  </si>
-  <si>
-    <t>Lecture 16: Testing</t>
-  </si>
-  <si>
-    <t>Lecture 17: Code Quality</t>
   </si>
   <si>
     <t>Lecture 1:
@@ -106,24 +91,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Lecture  15: ORM, Designing a Persistence Layer
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Lab 6: ORM
-(assigned)</t>
-    </r>
-  </si>
-  <si>
     <t>Exam</t>
   </si>
   <si>
@@ -160,14 +127,6 @@
     <t>Legend</t>
   </si>
   <si>
-    <t>A03: Team MS2
-50% Progress on Features</t>
-  </si>
-  <si>
-    <t>SQL/JDBC/ORM Review &amp; Labs
-(in class)</t>
-  </si>
-  <si>
     <t>A03: Team MS3
 75% Working System
 (w/SQL DB)</t>
@@ -206,9 +165,6 @@
 50% Progresss</t>
   </si>
   <si>
-    <t>A04: Individual MS3 Final Project Demo</t>
-  </si>
-  <si>
     <t>FINAL EXAM PERIOD
 101: 8:00-10:00 102: 10:15-12:15
 A08: Team Presentation and Demonstration
@@ -239,51 +195,6 @@
 A11: Team Project
 Final Self/Peer Evaluations due
 both 7:00 am (Marmoset)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Lecture 14: DB Applications, JDBC
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Lab 4: SQL
-due (7:00a)</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Lab 5: JDBC
-(assigned)</t>
-    </r>
-  </si>
-  <si>
-    <t>Work Ethic Lecture</t>
   </si>
   <si>
     <t>Final Presentation &amp; Demo</t>
@@ -450,26 +361,92 @@
 (Marmoset)</t>
   </si>
   <si>
-    <t>CS320: SW Engineering - Spring 2020 Schedule
-(as of 3-12-2020, subject to change)</t>
+    <t>A09: Individual Project Report due 7:00 am
+(Marmoset)</t>
+  </si>
+  <si>
+    <t>A08: Team Technical Report due 7:00 am
+(Marmoset)</t>
+  </si>
+  <si>
+    <t>Lab 4: SQL
+due (7:00a)</t>
+  </si>
+  <si>
+    <t>A03: Team MS1
+Minimal Working System
+PPT: Team Drive
+Code: Marmoset
+due (7:00a)</t>
+  </si>
+  <si>
+    <t>Coronavirus Closure</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Lectures 14 &amp; 15: DB Applications, JDBC / ORM
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Lab 5: JDBC
+Lab 6: ORM
+(assigned)</t>
+    </r>
+  </si>
+  <si>
+    <t>Lecture  15: ORM, Designing a Persistence Layer
+SQL/JDBC/ORM Review &amp; Labs
+(on-line)</t>
+  </si>
+  <si>
+    <t>SQL/JDBC/ORM Review &amp; Labs
+(on-line)</t>
+  </si>
+  <si>
+    <t>Lecture 16: Testing
+(on-line)</t>
+  </si>
+  <si>
+    <t>Lecture 17: Code Quality
+(on-line)</t>
   </si>
   <si>
     <t>Library Project Example
 Analysis &amp;
-Review</t>
+Review
+(on-line)</t>
+  </si>
+  <si>
+    <t>Mid-Term
+Exam
+(on-line)</t>
+  </si>
+  <si>
+    <t>A03: Team MS2
+50% Progress on Features
+(on-line)</t>
   </si>
   <si>
     <t>Exam Review
 and
-Library Project Example Review</t>
-  </si>
-  <si>
-    <t>A09: Individual Project Report due 7:00 am
-(Marmoset)</t>
-  </si>
-  <si>
-    <t>A08: Team Technical Report due 7:00 am
-(Marmoset)</t>
+Library Project Example Review
+(on-line)</t>
+  </si>
+  <si>
+    <t>A04: Individual MS3 Final Project Demo
+(on-line)</t>
+  </si>
+  <si>
+    <t>CS320: SW Engineering - Spring 2020 Schedule
+(as of 3-22-2020, subject to change)</t>
   </si>
 </sst>
 </file>
@@ -1118,7 +1095,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="135">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1399,21 +1376,12 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1444,9 +1412,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1462,8 +1427,47 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -1471,56 +1475,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1831,8 +1802,8 @@
   </sheetPr>
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J49" sqref="J49"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1850,21 +1821,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="57.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="127" t="s">
-        <v>65</v>
-      </c>
-      <c r="B1" s="128"/>
-      <c r="C1" s="128"/>
-      <c r="D1" s="128"/>
-      <c r="E1" s="128"/>
-      <c r="F1" s="128"/>
-      <c r="G1" s="128"/>
-      <c r="H1" s="128"/>
-      <c r="I1" s="129"/>
+      <c r="A1" s="111" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="112"/>
+      <c r="C1" s="112"/>
+      <c r="D1" s="112"/>
+      <c r="E1" s="112"/>
+      <c r="F1" s="112"/>
+      <c r="G1" s="112"/>
+      <c r="H1" s="112"/>
+      <c r="I1" s="113"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="113" t="s">
-        <v>31</v>
+      <c r="A2" s="109" t="s">
+        <v>26</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
@@ -1890,10 +1861,10 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="123">
+      <c r="A3" s="117">
         <v>16</v>
       </c>
-      <c r="B3" s="118" t="s">
+      <c r="B3" s="120" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="49">
@@ -1925,8 +1896,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="70.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="121"/>
-      <c r="B4" s="119"/>
+      <c r="A4" s="116"/>
+      <c r="B4" s="121"/>
       <c r="C4" s="47" t="s">
         <v>8</v>
       </c>
@@ -1937,19 +1908,19 @@
         <v>8</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G4" s="8"/>
       <c r="H4" s="80" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="I4" s="84"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="121">
+      <c r="A5" s="116">
         <v>15</v>
       </c>
-      <c r="B5" s="119"/>
+      <c r="B5" s="121"/>
       <c r="C5" s="10">
         <f>I3 + 1</f>
         <v>26</v>
@@ -1974,34 +1945,34 @@
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="I5" s="104">
+      <c r="I5" s="101">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="90.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="124"/>
-      <c r="B6" s="119"/>
+      <c r="A6" s="118"/>
+      <c r="B6" s="121"/>
       <c r="C6" s="79" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="D6" s="80" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="E6" s="81"/>
-      <c r="F6" s="110" t="s">
-        <v>57</v>
+      <c r="F6" s="106" t="s">
+        <v>47</v>
       </c>
       <c r="G6" s="8"/>
-      <c r="H6" s="107" t="s">
-        <v>58</v>
-      </c>
-      <c r="I6" s="114"/>
+      <c r="H6" s="104" t="s">
+        <v>48</v>
+      </c>
+      <c r="I6" s="110"/>
     </row>
     <row r="7" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="123">
+      <c r="A7" s="117">
         <v>14</v>
       </c>
-      <c r="B7" s="132" t="s">
+      <c r="B7" s="122" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="82">
@@ -2034,29 +2005,29 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="122"/>
-      <c r="B8" s="133"/>
+      <c r="A8" s="119"/>
+      <c r="B8" s="123"/>
       <c r="C8" s="46" t="s">
-        <v>63</v>
-      </c>
-      <c r="D8" s="105" t="s">
-        <v>62</v>
+        <v>53</v>
+      </c>
+      <c r="D8" s="102" t="s">
+        <v>52</v>
       </c>
       <c r="E8" s="27"/>
       <c r="F8" s="27" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="G8" s="78"/>
       <c r="H8" s="72" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="I8" s="42"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="131">
+      <c r="A9" s="115">
         <v>13</v>
       </c>
-      <c r="B9" s="133"/>
+      <c r="B9" s="123"/>
       <c r="C9" s="18">
         <f>I7 + 1</f>
         <v>9</v>
@@ -2087,29 +2058,29 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="121"/>
-      <c r="B10" s="133"/>
+      <c r="A10" s="116"/>
+      <c r="B10" s="123"/>
       <c r="C10" s="46" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="D10" s="72" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E10" s="15"/>
       <c r="F10" s="14" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="G10" s="15"/>
       <c r="H10" s="16" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="I10" s="17"/>
     </row>
     <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="121">
+      <c r="A11" s="116">
         <v>12</v>
       </c>
-      <c r="B11" s="133"/>
+      <c r="B11" s="123"/>
       <c r="C11" s="21">
         <f>I9 + 1</f>
         <v>16</v>
@@ -2140,27 +2111,27 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="121"/>
-      <c r="B12" s="133"/>
+      <c r="A12" s="116"/>
+      <c r="B12" s="123"/>
       <c r="C12" s="43"/>
       <c r="D12" s="37" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="E12" s="15"/>
       <c r="F12" s="27" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="G12" s="15"/>
       <c r="H12" s="16" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="I12" s="85"/>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="121">
+      <c r="A13" s="116">
         <v>11</v>
       </c>
-      <c r="B13" s="133"/>
+      <c r="B13" s="123"/>
       <c r="C13" s="21">
         <f>I11 + 1</f>
         <v>23</v>
@@ -2191,29 +2162,29 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="97.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="122"/>
-      <c r="B14" s="133"/>
+      <c r="A14" s="119"/>
+      <c r="B14" s="123"/>
       <c r="C14" s="43"/>
-      <c r="D14" s="105" t="s">
-        <v>54</v>
+      <c r="D14" s="102" t="s">
+        <v>44</v>
       </c>
       <c r="E14" s="87"/>
       <c r="F14" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="G14" s="103"/>
-      <c r="H14" s="108" t="s">
-        <v>17</v>
+        <v>33</v>
+      </c>
+      <c r="G14" s="100"/>
+      <c r="H14" s="105" t="s">
+        <v>15</v>
       </c>
       <c r="I14" s="57" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="123">
+      <c r="A15" s="117">
         <v>10</v>
       </c>
-      <c r="B15" s="132" t="s">
+      <c r="B15" s="122" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="49">
@@ -2245,8 +2216,8 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="124"/>
-      <c r="B16" s="134"/>
+      <c r="A16" s="118"/>
+      <c r="B16" s="124"/>
       <c r="C16" s="54" t="str">
         <f>I14</f>
         <v>WINTER BREAK</v>
@@ -2271,8 +2242,8 @@
         <f>G16</f>
         <v>WINTER BREAK</v>
       </c>
-      <c r="I16" s="111" t="s">
-        <v>60</v>
+      <c r="I16" s="107" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="35" customFormat="1" ht="21.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -2291,7 +2262,7 @@
       <c r="B18" s="31"/>
       <c r="D18" s="34"/>
       <c r="E18" s="70" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F18" s="34"/>
       <c r="G18" s="34"/>
@@ -2303,7 +2274,7 @@
       <c r="B19" s="36"/>
       <c r="D19" s="30"/>
       <c r="E19" s="64" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F19" s="30"/>
       <c r="G19" s="30"/>
@@ -2315,7 +2286,7 @@
       <c r="B20" s="31"/>
       <c r="D20" s="34"/>
       <c r="E20" s="65" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="F20" s="34"/>
       <c r="G20" s="34"/>
@@ -2327,7 +2298,7 @@
       <c r="B21" s="31"/>
       <c r="D21" s="34"/>
       <c r="E21" s="66" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F21" s="34"/>
       <c r="G21" s="34"/>
@@ -2339,7 +2310,7 @@
       <c r="B22" s="31"/>
       <c r="D22" s="34"/>
       <c r="E22" s="67" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F22" s="34"/>
       <c r="G22" s="34"/>
@@ -2352,7 +2323,7 @@
       <c r="C23" s="62"/>
       <c r="D23" s="34"/>
       <c r="E23" s="68" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F23" s="34"/>
       <c r="G23" s="34"/>
@@ -2382,19 +2353,19 @@
       <c r="I25" s="30"/>
     </row>
     <row r="26" spans="1:9" s="32" customFormat="1" ht="57.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="127" t="str">
+      <c r="A26" s="111" t="str">
         <f>A1</f>
         <v>CS320: SW Engineering - Spring 2020 Schedule
-(as of 3-12-2020, subject to change)</v>
-      </c>
-      <c r="B26" s="128"/>
-      <c r="C26" s="128"/>
-      <c r="D26" s="128"/>
-      <c r="E26" s="128"/>
-      <c r="F26" s="128"/>
-      <c r="G26" s="128"/>
-      <c r="H26" s="128"/>
-      <c r="I26" s="129"/>
+(as of 3-22-2020, subject to change)</v>
+      </c>
+      <c r="B26" s="112"/>
+      <c r="C26" s="112"/>
+      <c r="D26" s="112"/>
+      <c r="E26" s="112"/>
+      <c r="F26" s="112"/>
+      <c r="G26" s="112"/>
+      <c r="H26" s="112"/>
+      <c r="I26" s="113"/>
     </row>
     <row r="27" spans="1:9" s="2" customFormat="1" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="str">
@@ -2432,7 +2403,7 @@
       </c>
     </row>
     <row r="28" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="130">
+      <c r="A28" s="114">
         <v>10</v>
       </c>
       <c r="B28" s="73"/>
@@ -2466,8 +2437,8 @@
       </c>
     </row>
     <row r="29" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="131"/>
-      <c r="B29" s="119" t="s">
+      <c r="A29" s="115"/>
+      <c r="B29" s="121" t="s">
         <v>13</v>
       </c>
       <c r="C29" s="47" t="str">
@@ -2501,10 +2472,10 @@
       </c>
     </row>
     <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="131">
+      <c r="A30" s="115">
         <v>9</v>
       </c>
-      <c r="B30" s="119"/>
+      <c r="B30" s="121"/>
       <c r="C30" s="90">
         <f>I15 + 1</f>
         <v>8</v>
@@ -2535,30 +2506,32 @@
       </c>
     </row>
     <row r="31" spans="1:9" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="121"/>
-      <c r="B31" s="119"/>
+      <c r="A31" s="116"/>
+      <c r="B31" s="121"/>
       <c r="C31" s="91" t="str">
         <f>H29</f>
         <v>WINTER BREAK</v>
       </c>
       <c r="D31" s="37" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="E31" s="7"/>
       <c r="F31" s="24" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G31" s="7"/>
-      <c r="H31" s="105" t="s">
-        <v>50</v>
-      </c>
-      <c r="I31" s="71"/>
+      <c r="H31" s="102" t="s">
+        <v>60</v>
+      </c>
+      <c r="I31" s="45" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="32" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="121">
+      <c r="A32" s="116">
         <v>8</v>
       </c>
-      <c r="B32" s="119"/>
+      <c r="B32" s="121"/>
       <c r="C32" s="25">
         <f>I30 + 1</f>
         <v>15</v>
@@ -2589,29 +2562,29 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="121"/>
-      <c r="B33" s="119"/>
+      <c r="A33" s="116"/>
+      <c r="B33" s="121"/>
       <c r="C33" s="10"/>
-      <c r="D33" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="E33" s="7"/>
+      <c r="D33" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E33" s="28" t="s">
+        <v>58</v>
+      </c>
       <c r="F33" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G33" s="96" t="s">
-        <v>46</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="G33" s="7"/>
       <c r="H33" s="7" t="s">
-        <v>34</v>
+        <v>61</v>
       </c>
       <c r="I33" s="71"/>
     </row>
     <row r="34" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="121">
+      <c r="A34" s="116">
         <v>7</v>
       </c>
-      <c r="B34" s="119"/>
+      <c r="B34" s="121"/>
       <c r="C34" s="10">
         <f>I32 + 1</f>
         <v>22</v>
@@ -2642,26 +2615,26 @@
       </c>
     </row>
     <row r="35" spans="1:9" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="121"/>
-      <c r="B35" s="119"/>
-      <c r="C35" s="10"/>
+      <c r="A35" s="116"/>
+      <c r="B35" s="121"/>
+      <c r="C35" s="46" t="s">
+        <v>38</v>
+      </c>
       <c r="D35" s="7" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
       <c r="E35" s="7"/>
       <c r="F35" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G35" s="69" t="s">
-        <v>47</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="G35" s="7"/>
       <c r="H35" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="I35" s="42"/>
+        <v>62</v>
+      </c>
+      <c r="I35" s="71"/>
     </row>
     <row r="36" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="121">
+      <c r="A36" s="116">
         <v>6</v>
       </c>
       <c r="B36" s="74"/>
@@ -2680,50 +2653,52 @@
       <c r="F36" s="76">
         <v>1</v>
       </c>
-      <c r="G36" s="100">
+      <c r="G36" s="97">
         <f t="shared" si="7"/>
         <v>2</v>
       </c>
-      <c r="H36" s="83">
+      <c r="H36" s="97">
         <f t="shared" si="7"/>
         <v>3</v>
       </c>
-      <c r="I36" s="101">
+      <c r="I36" s="98">
         <f>H36 + 1</f>
         <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="69.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="124"/>
+      <c r="A37" s="118"/>
       <c r="B37" s="75"/>
-      <c r="C37" s="109"/>
-      <c r="D37" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="E37" s="111" t="s">
-        <v>48</v>
-      </c>
-      <c r="F37" s="72" t="s">
+      <c r="C37" s="130" t="s">
+        <v>39</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E37" s="104"/>
+      <c r="F37" s="131" t="s">
         <v>67</v>
       </c>
-      <c r="G37" s="41"/>
-      <c r="H37" s="94" t="s">
-        <v>15</v>
-      </c>
-      <c r="I37" s="42"/>
+      <c r="G37" s="27"/>
+      <c r="H37" s="72" t="s">
+        <v>68</v>
+      </c>
+      <c r="I37" s="45" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="38" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="123">
+      <c r="A38" s="117">
         <v>5</v>
       </c>
-      <c r="B38" s="116" t="s">
+      <c r="B38" s="125" t="s">
         <v>14</v>
       </c>
       <c r="C38" s="43">
         <f>I36 + 1</f>
         <v>5</v>
       </c>
-      <c r="D38" s="102">
+      <c r="D38" s="99">
         <f>C38 + 1</f>
         <v>6</v>
       </c>
@@ -2749,31 +2724,31 @@
       </c>
     </row>
     <row r="39" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="121"/>
-      <c r="B39" s="117"/>
-      <c r="C39" s="43"/>
-      <c r="D39" s="98" t="s">
-        <v>43</v>
+      <c r="A39" s="116"/>
+      <c r="B39" s="126"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="132" t="s">
+        <v>66</v>
       </c>
       <c r="E39" s="41"/>
-      <c r="F39" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="G39" s="115" t="s">
-        <v>68</v>
-      </c>
-      <c r="H39" s="48" t="s">
+      <c r="F39" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="G39" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="I39" s="52" t="s">
+      <c r="H39" s="60" t="s">
         <v>6</v>
       </c>
+      <c r="I39" s="45" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="40" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="121">
+      <c r="A40" s="116">
         <v>4</v>
       </c>
-      <c r="B40" s="117"/>
+      <c r="B40" s="126"/>
       <c r="C40" s="48">
         <f>I38 + 1</f>
         <v>12</v>
@@ -2804,8 +2779,8 @@
       </c>
     </row>
     <row r="41" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="121"/>
-      <c r="B41" s="117"/>
+      <c r="A41" s="116"/>
+      <c r="B41" s="126"/>
       <c r="C41" s="47" t="s">
         <v>6</v>
       </c>
@@ -2813,7 +2788,7 @@
         <v>6</v>
       </c>
       <c r="E41" s="15"/>
-      <c r="F41" s="95" t="s">
+      <c r="F41" s="27" t="s">
         <v>7</v>
       </c>
       <c r="G41" s="27"/>
@@ -2823,10 +2798,10 @@
       <c r="I41" s="42"/>
     </row>
     <row r="42" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="121">
+      <c r="A42" s="116">
         <v>3</v>
       </c>
-      <c r="B42" s="117"/>
+      <c r="B42" s="126"/>
       <c r="C42" s="43">
         <f>I40 + 1</f>
         <v>19</v>
@@ -2857,27 +2832,27 @@
       </c>
     </row>
     <row r="43" spans="1:9" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="121"/>
-      <c r="B43" s="117"/>
+      <c r="A43" s="116"/>
+      <c r="B43" s="126"/>
       <c r="C43" s="43"/>
       <c r="D43" s="92" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="E43" s="15"/>
-      <c r="F43" s="95" t="s">
+      <c r="F43" s="94" t="s">
         <v>7</v>
       </c>
       <c r="G43" s="87"/>
-      <c r="H43" s="95" t="s">
+      <c r="H43" s="94" t="s">
         <v>7</v>
       </c>
       <c r="I43" s="85"/>
     </row>
     <row r="44" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="121">
+      <c r="A44" s="116">
         <v>2</v>
       </c>
-      <c r="B44" s="117"/>
+      <c r="B44" s="126"/>
       <c r="C44" s="21">
         <f>I42 + 1</f>
         <v>26</v>
@@ -2898,7 +2873,7 @@
         <f t="shared" ref="G44" si="12">F44 + 1</f>
         <v>30</v>
       </c>
-      <c r="H44" s="99">
+      <c r="H44" s="96">
         <v>1</v>
       </c>
       <c r="I44" s="6">
@@ -2907,27 +2882,27 @@
       </c>
     </row>
     <row r="45" spans="1:9" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="124"/>
-      <c r="B45" s="117"/>
-      <c r="C45" s="97"/>
-      <c r="D45" s="108" t="s">
+      <c r="A45" s="118"/>
+      <c r="B45" s="126"/>
+      <c r="C45" s="95"/>
+      <c r="D45" s="105" t="s">
         <v>7</v>
       </c>
-      <c r="E45" s="103"/>
-      <c r="F45" s="108" t="s">
+      <c r="E45" s="100"/>
+      <c r="F45" s="105" t="s">
         <v>7</v>
       </c>
-      <c r="G45" s="106"/>
+      <c r="G45" s="103"/>
       <c r="H45" s="24" t="s">
         <v>7</v>
       </c>
       <c r="I45" s="9"/>
     </row>
     <row r="46" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="123">
+      <c r="A46" s="117">
         <v>1</v>
       </c>
-      <c r="B46" s="118" t="s">
+      <c r="B46" s="120" t="s">
         <v>5</v>
       </c>
       <c r="C46" s="38">
@@ -2938,7 +2913,7 @@
         <f t="shared" ref="D46:I46" si="13">C46 + 1</f>
         <v>4</v>
       </c>
-      <c r="E46" s="99">
+      <c r="E46" s="96">
         <f t="shared" si="13"/>
         <v>5</v>
       </c>
@@ -2960,8 +2935,8 @@
       </c>
     </row>
     <row r="47" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="121"/>
-      <c r="B47" s="119"/>
+      <c r="A47" s="116"/>
+      <c r="B47" s="121"/>
       <c r="C47" s="39"/>
       <c r="D47" s="7" t="s">
         <v>7</v>
@@ -2971,18 +2946,18 @@
         <v>7</v>
       </c>
       <c r="G47" s="44"/>
-      <c r="H47" s="112" t="s">
-        <v>55</v>
+      <c r="H47" s="108" t="s">
+        <v>45</v>
       </c>
       <c r="I47" s="45" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="125" t="s">
-        <v>52</v>
-      </c>
-      <c r="B48" s="119"/>
+      <c r="A48" s="128" t="s">
+        <v>42</v>
+      </c>
+      <c r="B48" s="121"/>
       <c r="C48" s="25">
         <f>I46 + 1</f>
         <v>10</v>
@@ -3013,17 +2988,17 @@
       </c>
     </row>
     <row r="49" spans="1:9" ht="144" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="126"/>
-      <c r="B49" s="120"/>
+      <c r="A49" s="129"/>
+      <c r="B49" s="127"/>
       <c r="C49" s="69" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D49" s="29" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="E49" s="26"/>
       <c r="F49" s="29" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="G49" s="26"/>
       <c r="H49" s="12"/>
@@ -3032,6 +3007,19 @@
     <row r="50" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="B38:B45"/>
+    <mergeCell ref="B46:B49"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A40:A41"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A28:A29"/>
     <mergeCell ref="A30:A31"/>
@@ -3045,19 +3033,6 @@
     <mergeCell ref="A26:I26"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="B29:B35"/>
-    <mergeCell ref="B38:B45"/>
-    <mergeCell ref="B46:B49"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A40:A41"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated lab06 due date
</commit_message>
<xml_diff>
--- a/CS320-Spring2020Calendar.xlsx
+++ b/CS320-Spring2020Calendar.xlsx
@@ -180,9 +180,6 @@
     <t>Lab 5: JDBC due
 7:00 am
 (Marmoset)</t>
-  </si>
-  <si>
-    <t>Lab 6: ORM due  7:00 am (Marmoset)</t>
   </si>
   <si>
     <t>A11: Team Project Midterm
@@ -447,6 +444,11 @@
   <si>
     <t>CS320: SW Engineering - Spring 2020 Schedule
 (as of 3-22-2020, subject to change)</t>
+  </si>
+  <si>
+    <t>Lab 6: ORM due  Monday, 3-30-20 by 7:00 am
+----------&gt;&gt;&gt;
+ (Marmoset)</t>
   </si>
 </sst>
 </file>
@@ -1427,32 +1429,20 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -1460,6 +1450,42 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1468,30 +1494,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1802,8 +1804,8 @@
   </sheetPr>
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1821,17 +1823,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="57.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="111" t="s">
-        <v>70</v>
-      </c>
-      <c r="B1" s="112"/>
-      <c r="C1" s="112"/>
-      <c r="D1" s="112"/>
-      <c r="E1" s="112"/>
-      <c r="F1" s="112"/>
-      <c r="G1" s="112"/>
-      <c r="H1" s="112"/>
-      <c r="I1" s="113"/>
+      <c r="A1" s="125" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="126"/>
+      <c r="C1" s="126"/>
+      <c r="D1" s="126"/>
+      <c r="E1" s="126"/>
+      <c r="F1" s="126"/>
+      <c r="G1" s="126"/>
+      <c r="H1" s="126"/>
+      <c r="I1" s="127"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="109" t="s">
@@ -1861,10 +1863,10 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="117">
+      <c r="A3" s="121">
         <v>16</v>
       </c>
-      <c r="B3" s="120" t="s">
+      <c r="B3" s="116" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="49">
@@ -1896,8 +1898,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="70.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="116"/>
-      <c r="B4" s="121"/>
+      <c r="A4" s="119"/>
+      <c r="B4" s="117"/>
       <c r="C4" s="47" t="s">
         <v>8</v>
       </c>
@@ -1912,15 +1914,15 @@
       </c>
       <c r="G4" s="8"/>
       <c r="H4" s="80" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I4" s="84"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="116">
+      <c r="A5" s="119">
         <v>15</v>
       </c>
-      <c r="B5" s="121"/>
+      <c r="B5" s="117"/>
       <c r="C5" s="10">
         <f>I3 + 1</f>
         <v>26</v>
@@ -1950,29 +1952,29 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="90.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="118"/>
-      <c r="B6" s="121"/>
+      <c r="A6" s="122"/>
+      <c r="B6" s="117"/>
       <c r="C6" s="79" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D6" s="80" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E6" s="81"/>
       <c r="F6" s="106" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G6" s="8"/>
       <c r="H6" s="104" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I6" s="110"/>
     </row>
     <row r="7" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="117">
+      <c r="A7" s="121">
         <v>14</v>
       </c>
-      <c r="B7" s="122" t="s">
+      <c r="B7" s="130" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="82">
@@ -2005,17 +2007,17 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="119"/>
-      <c r="B8" s="123"/>
+      <c r="A8" s="120"/>
+      <c r="B8" s="131"/>
       <c r="C8" s="46" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D8" s="102" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E8" s="27"/>
       <c r="F8" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G8" s="78"/>
       <c r="H8" s="72" t="s">
@@ -2024,10 +2026,10 @@
       <c r="I8" s="42"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="115">
+      <c r="A9" s="129">
         <v>13</v>
       </c>
-      <c r="B9" s="123"/>
+      <c r="B9" s="131"/>
       <c r="C9" s="18">
         <f>I7 + 1</f>
         <v>9</v>
@@ -2058,10 +2060,10 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="116"/>
-      <c r="B10" s="123"/>
+      <c r="A10" s="119"/>
+      <c r="B10" s="131"/>
       <c r="C10" s="46" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D10" s="72" t="s">
         <v>30</v>
@@ -2077,10 +2079,10 @@
       <c r="I10" s="17"/>
     </row>
     <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="116">
+      <c r="A11" s="119">
         <v>12</v>
       </c>
-      <c r="B11" s="123"/>
+      <c r="B11" s="131"/>
       <c r="C11" s="21">
         <f>I9 + 1</f>
         <v>16</v>
@@ -2111,8 +2113,8 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="116"/>
-      <c r="B12" s="123"/>
+      <c r="A12" s="119"/>
+      <c r="B12" s="131"/>
       <c r="C12" s="43"/>
       <c r="D12" s="37" t="s">
         <v>29</v>
@@ -2128,10 +2130,10 @@
       <c r="I12" s="85"/>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="116">
+      <c r="A13" s="119">
         <v>11</v>
       </c>
-      <c r="B13" s="123"/>
+      <c r="B13" s="131"/>
       <c r="C13" s="21">
         <f>I11 + 1</f>
         <v>23</v>
@@ -2162,11 +2164,11 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="97.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="119"/>
-      <c r="B14" s="123"/>
+      <c r="A14" s="120"/>
+      <c r="B14" s="131"/>
       <c r="C14" s="43"/>
       <c r="D14" s="102" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E14" s="87"/>
       <c r="F14" s="40" t="s">
@@ -2181,10 +2183,10 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="117">
+      <c r="A15" s="121">
         <v>10</v>
       </c>
-      <c r="B15" s="122" t="s">
+      <c r="B15" s="130" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="49">
@@ -2216,8 +2218,8 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="118"/>
-      <c r="B16" s="124"/>
+      <c r="A16" s="122"/>
+      <c r="B16" s="132"/>
       <c r="C16" s="54" t="str">
         <f>I14</f>
         <v>WINTER BREAK</v>
@@ -2243,7 +2245,7 @@
         <v>WINTER BREAK</v>
       </c>
       <c r="I16" s="107" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="35" customFormat="1" ht="21.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -2353,19 +2355,19 @@
       <c r="I25" s="30"/>
     </row>
     <row r="26" spans="1:9" s="32" customFormat="1" ht="57.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="111" t="str">
+      <c r="A26" s="125" t="str">
         <f>A1</f>
         <v>CS320: SW Engineering - Spring 2020 Schedule
 (as of 3-22-2020, subject to change)</v>
       </c>
-      <c r="B26" s="112"/>
-      <c r="C26" s="112"/>
-      <c r="D26" s="112"/>
-      <c r="E26" s="112"/>
-      <c r="F26" s="112"/>
-      <c r="G26" s="112"/>
-      <c r="H26" s="112"/>
-      <c r="I26" s="113"/>
+      <c r="B26" s="126"/>
+      <c r="C26" s="126"/>
+      <c r="D26" s="126"/>
+      <c r="E26" s="126"/>
+      <c r="F26" s="126"/>
+      <c r="G26" s="126"/>
+      <c r="H26" s="126"/>
+      <c r="I26" s="127"/>
     </row>
     <row r="27" spans="1:9" s="2" customFormat="1" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="str">
@@ -2403,7 +2405,7 @@
       </c>
     </row>
     <row r="28" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="114">
+      <c r="A28" s="128">
         <v>10</v>
       </c>
       <c r="B28" s="73"/>
@@ -2437,8 +2439,8 @@
       </c>
     </row>
     <row r="29" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="115"/>
-      <c r="B29" s="121" t="s">
+      <c r="A29" s="129"/>
+      <c r="B29" s="117" t="s">
         <v>13</v>
       </c>
       <c r="C29" s="47" t="str">
@@ -2472,10 +2474,10 @@
       </c>
     </row>
     <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="115">
+      <c r="A30" s="129">
         <v>9</v>
       </c>
-      <c r="B30" s="121"/>
+      <c r="B30" s="117"/>
       <c r="C30" s="90">
         <f>I15 + 1</f>
         <v>8</v>
@@ -2506,8 +2508,8 @@
       </c>
     </row>
     <row r="31" spans="1:9" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="116"/>
-      <c r="B31" s="121"/>
+      <c r="A31" s="119"/>
+      <c r="B31" s="117"/>
       <c r="C31" s="91" t="str">
         <f>H29</f>
         <v>WINTER BREAK</v>
@@ -2521,17 +2523,17 @@
       </c>
       <c r="G31" s="7"/>
       <c r="H31" s="102" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I31" s="45" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="116">
+      <c r="A32" s="119">
         <v>8</v>
       </c>
-      <c r="B32" s="121"/>
+      <c r="B32" s="117"/>
       <c r="C32" s="25">
         <f>I30 + 1</f>
         <v>15</v>
@@ -2562,29 +2564,29 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="116"/>
-      <c r="B33" s="121"/>
+      <c r="A33" s="119"/>
+      <c r="B33" s="117"/>
       <c r="C33" s="10"/>
       <c r="D33" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E33" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="F33" s="7" t="s">
         <v>58</v>
-      </c>
-      <c r="F33" s="7" t="s">
-        <v>59</v>
       </c>
       <c r="G33" s="7"/>
       <c r="H33" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I33" s="71"/>
     </row>
     <row r="34" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="116">
+      <c r="A34" s="119">
         <v>7</v>
       </c>
-      <c r="B34" s="121"/>
+      <c r="B34" s="117"/>
       <c r="C34" s="10">
         <f>I32 + 1</f>
         <v>22</v>
@@ -2615,26 +2617,26 @@
       </c>
     </row>
     <row r="35" spans="1:9" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="116"/>
-      <c r="B35" s="121"/>
+      <c r="A35" s="119"/>
+      <c r="B35" s="117"/>
       <c r="C35" s="46" t="s">
         <v>38</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E35" s="7"/>
       <c r="F35" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G35" s="7"/>
       <c r="H35" s="24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I35" s="71"/>
     </row>
     <row r="36" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="116">
+      <c r="A36" s="119">
         <v>6</v>
       </c>
       <c r="B36" s="74"/>
@@ -2667,31 +2669,31 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="69.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="118"/>
+      <c r="A37" s="122"/>
       <c r="B37" s="75"/>
-      <c r="C37" s="130" t="s">
-        <v>39</v>
+      <c r="C37" s="111" t="s">
+        <v>70</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E37" s="104"/>
-      <c r="F37" s="131" t="s">
-        <v>67</v>
+      <c r="F37" s="112" t="s">
+        <v>66</v>
       </c>
       <c r="G37" s="27"/>
       <c r="H37" s="72" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I37" s="45" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="117">
+      <c r="A38" s="121">
         <v>5</v>
       </c>
-      <c r="B38" s="125" t="s">
+      <c r="B38" s="114" t="s">
         <v>14</v>
       </c>
       <c r="C38" s="43">
@@ -2724,15 +2726,15 @@
       </c>
     </row>
     <row r="39" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="116"/>
-      <c r="B39" s="126"/>
+      <c r="A39" s="119"/>
+      <c r="B39" s="115"/>
       <c r="C39" s="27"/>
-      <c r="D39" s="132" t="s">
-        <v>66</v>
+      <c r="D39" s="113" t="s">
+        <v>65</v>
       </c>
       <c r="E39" s="41"/>
       <c r="F39" s="37" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G39" s="60" t="s">
         <v>6</v>
@@ -2741,14 +2743,14 @@
         <v>6</v>
       </c>
       <c r="I39" s="45" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="116">
+      <c r="A40" s="119">
         <v>4</v>
       </c>
-      <c r="B40" s="126"/>
+      <c r="B40" s="115"/>
       <c r="C40" s="48">
         <f>I38 + 1</f>
         <v>12</v>
@@ -2779,8 +2781,8 @@
       </c>
     </row>
     <row r="41" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="116"/>
-      <c r="B41" s="126"/>
+      <c r="A41" s="119"/>
+      <c r="B41" s="115"/>
       <c r="C41" s="47" t="s">
         <v>6</v>
       </c>
@@ -2798,10 +2800,10 @@
       <c r="I41" s="42"/>
     </row>
     <row r="42" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="116">
+      <c r="A42" s="119">
         <v>3</v>
       </c>
-      <c r="B42" s="126"/>
+      <c r="B42" s="115"/>
       <c r="C42" s="43">
         <f>I40 + 1</f>
         <v>19</v>
@@ -2832,8 +2834,8 @@
       </c>
     </row>
     <row r="43" spans="1:9" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="116"/>
-      <c r="B43" s="126"/>
+      <c r="A43" s="119"/>
+      <c r="B43" s="115"/>
       <c r="C43" s="43"/>
       <c r="D43" s="92" t="s">
         <v>28</v>
@@ -2849,10 +2851,10 @@
       <c r="I43" s="85"/>
     </row>
     <row r="44" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="116">
+      <c r="A44" s="119">
         <v>2</v>
       </c>
-      <c r="B44" s="126"/>
+      <c r="B44" s="115"/>
       <c r="C44" s="21">
         <f>I42 + 1</f>
         <v>26</v>
@@ -2882,8 +2884,8 @@
       </c>
     </row>
     <row r="45" spans="1:9" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="118"/>
-      <c r="B45" s="126"/>
+      <c r="A45" s="122"/>
+      <c r="B45" s="115"/>
       <c r="C45" s="95"/>
       <c r="D45" s="105" t="s">
         <v>7</v>
@@ -2899,10 +2901,10 @@
       <c r="I45" s="9"/>
     </row>
     <row r="46" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="117">
+      <c r="A46" s="121">
         <v>1</v>
       </c>
-      <c r="B46" s="120" t="s">
+      <c r="B46" s="116" t="s">
         <v>5</v>
       </c>
       <c r="C46" s="38">
@@ -2935,8 +2937,8 @@
       </c>
     </row>
     <row r="47" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="116"/>
-      <c r="B47" s="121"/>
+      <c r="A47" s="119"/>
+      <c r="B47" s="117"/>
       <c r="C47" s="39"/>
       <c r="D47" s="7" t="s">
         <v>7</v>
@@ -2947,17 +2949,17 @@
       </c>
       <c r="G47" s="44"/>
       <c r="H47" s="108" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I47" s="45" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="128" t="s">
-        <v>42</v>
-      </c>
-      <c r="B48" s="121"/>
+      <c r="A48" s="123" t="s">
+        <v>41</v>
+      </c>
+      <c r="B48" s="117"/>
       <c r="C48" s="25">
         <f>I46 + 1</f>
         <v>10</v>
@@ -2988,10 +2990,10 @@
       </c>
     </row>
     <row r="49" spans="1:9" ht="144" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="129"/>
-      <c r="B49" s="127"/>
+      <c r="A49" s="124"/>
+      <c r="B49" s="118"/>
       <c r="C49" s="69" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D49" s="29" t="s">
         <v>37</v>
@@ -3007,6 +3009,19 @@
     <row r="50" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="B7:B14"/>
+    <mergeCell ref="A26:I26"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B29:B35"/>
     <mergeCell ref="B38:B45"/>
     <mergeCell ref="B46:B49"/>
     <mergeCell ref="A13:A14"/>
@@ -3020,19 +3035,6 @@
     <mergeCell ref="A36:A37"/>
     <mergeCell ref="A38:A39"/>
     <mergeCell ref="A40:A41"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="B7:B14"/>
-    <mergeCell ref="A26:I26"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B29:B35"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated calendar for TeamMS3
</commit_message>
<xml_diff>
--- a/CS320-Spring2020Calendar.xlsx
+++ b/CS320-Spring2020Calendar.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="72">
   <si>
     <t>Monday</t>
   </si>
@@ -37,10 +37,6 @@
   </si>
   <si>
     <t>SPRING BREAK</t>
-  </si>
-  <si>
-    <t>Team Session
-(in class)</t>
   </si>
   <si>
     <t>SEMESTER
@@ -127,11 +123,6 @@
     <t>Legend</t>
   </si>
   <si>
-    <t>A03: Team MS3
-75% Working System
-(w/SQL DB)</t>
-  </si>
-  <si>
     <t>A04: Individual MS1 Baseline Prototype</t>
   </si>
   <si>
@@ -163,18 +154,6 @@
   <si>
     <t>A04: Individual MS2
 50% Progresss</t>
-  </si>
-  <si>
-    <t>FINAL EXAM PERIOD
-101: 8:00-10:00 102: 10:15-12:15
-A08: Team Presentation and Demonstration
-(in class)</t>
-  </si>
-  <si>
-    <t>FINAL EXAM PERIOD
-103: 3:00-5:00
-A08: Team Presentation and Demonstration
-(in class)</t>
   </si>
   <si>
     <t>Lab 5: JDBC due
@@ -377,9 +356,6 @@
 due (7:00a)</t>
   </si>
   <si>
-    <t>Coronavirus Closure</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Lectures 14 &amp; 15: DB Applications, JDBC / ORM
 </t>
@@ -399,56 +375,87 @@
     </r>
   </si>
   <si>
+    <t>Lab 6: ORM due  Monday, 3-30-20 by 7:00 am
+----------&gt;&gt;&gt;
+ (Marmoset)</t>
+  </si>
+  <si>
+    <t>CS320: SW Engineering - Spring 2020 Schedule
+(as of 4-7-2020, subject to change)</t>
+  </si>
+  <si>
+    <t>Team Project Work Session
+(Zoom)</t>
+  </si>
+  <si>
+    <t>Team Project
+Work Session
+(Zoom)</t>
+  </si>
+  <si>
     <t>Lecture  15: ORM, Designing a Persistence Layer
 SQL/JDBC/ORM Review &amp; Labs
-(on-line)</t>
+(Zoom)</t>
+  </si>
+  <si>
+    <t>Lecture 16: Testing
+(Zoom)</t>
+  </si>
+  <si>
+    <t>Lecture 17: Code Quality
+(Zoom)</t>
   </si>
   <si>
     <t>SQL/JDBC/ORM Review &amp; Labs
-(on-line)</t>
-  </si>
-  <si>
-    <t>Lecture 16: Testing
-(on-line)</t>
-  </si>
-  <si>
-    <t>Lecture 17: Code Quality
-(on-line)</t>
+(Zoom)</t>
   </si>
   <si>
     <t>Library Project Example
 Analysis &amp;
 Review
-(on-line)</t>
-  </si>
-  <si>
-    <t>Mid-Term
-Exam
-(on-line)</t>
-  </si>
-  <si>
-    <t>A03: Team MS2
-50% Progress on Features
-(on-line)</t>
+(Zoom)</t>
   </si>
   <si>
     <t>Exam Review
 and
 Library Project Example Review
-(on-line)</t>
+(Zoom)</t>
+  </si>
+  <si>
+    <t>Mid-Term
+Exam
+(take-at-home)</t>
   </si>
   <si>
     <t>A04: Individual MS3 Final Project Demo
-(on-line)</t>
-  </si>
-  <si>
-    <t>CS320: SW Engineering - Spring 2020 Schedule
-(as of 3-22-2020, subject to change)</t>
-  </si>
-  <si>
-    <t>Lab 6: ORM due  Monday, 3-30-20 by 7:00 am
-----------&gt;&gt;&gt;
- (Marmoset)</t>
+(Zoom)</t>
+  </si>
+  <si>
+    <t>FINAL EXAM PERIOD
+103: 3:00-5:00
+A08: Team Presentation and Demonstration
+(Zoom)</t>
+  </si>
+  <si>
+    <t>FINAL EXAM PERIOD
+101: 8:00-10:00 102: 10:15-12:15
+A08: Team Presentation and Demonstration
+(Zoom)</t>
+  </si>
+  <si>
+    <t>A03: Team MS2
+50% Progress on Features
+(Zoom)</t>
+  </si>
+  <si>
+    <t>Coronavirus Closure
+Preparing to
+teach on-line</t>
+  </si>
+  <si>
+    <t>A03: Team MS3
+75% Working System (SQL DB)
+(Zoom)</t>
   </si>
 </sst>
 </file>
@@ -1438,61 +1445,61 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1804,8 +1811,8 @@
   </sheetPr>
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1823,25 +1830,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="57.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="125" t="s">
-        <v>69</v>
-      </c>
-      <c r="B1" s="126"/>
-      <c r="C1" s="126"/>
-      <c r="D1" s="126"/>
-      <c r="E1" s="126"/>
-      <c r="F1" s="126"/>
-      <c r="G1" s="126"/>
-      <c r="H1" s="126"/>
-      <c r="I1" s="127"/>
+      <c r="A1" s="114" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="115"/>
+      <c r="G1" s="115"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="116"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="109" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>0</v>
@@ -1859,15 +1866,15 @@
         <v>4</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="120">
+        <v>16</v>
+      </c>
+      <c r="B3" s="123" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="121">
-        <v>16</v>
-      </c>
-      <c r="B3" s="116" t="s">
-        <v>11</v>
       </c>
       <c r="C3" s="49">
         <v>19</v>
@@ -1899,22 +1906,22 @@
     </row>
     <row r="4" spans="1:9" ht="70.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="119"/>
-      <c r="B4" s="117"/>
+      <c r="B4" s="124"/>
       <c r="C4" s="47" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" s="48" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="48" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G4" s="8"/>
       <c r="H4" s="80" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I4" s="84"/>
     </row>
@@ -1922,7 +1929,7 @@
       <c r="A5" s="119">
         <v>15</v>
       </c>
-      <c r="B5" s="117"/>
+      <c r="B5" s="124"/>
       <c r="C5" s="10">
         <f>I3 + 1</f>
         <v>26</v>
@@ -1952,30 +1959,30 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="90.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="122"/>
-      <c r="B6" s="117"/>
+      <c r="A6" s="121"/>
+      <c r="B6" s="124"/>
       <c r="C6" s="79" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D6" s="80" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E6" s="81"/>
       <c r="F6" s="106" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G6" s="8"/>
       <c r="H6" s="104" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="I6" s="110"/>
     </row>
     <row r="7" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="121">
+      <c r="A7" s="120">
         <v>14</v>
       </c>
-      <c r="B7" s="130" t="s">
-        <v>12</v>
+      <c r="B7" s="125" t="s">
+        <v>11</v>
       </c>
       <c r="C7" s="82">
         <f>I5 + 1</f>
@@ -2007,29 +2014,29 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="120"/>
-      <c r="B8" s="131"/>
+      <c r="A8" s="122"/>
+      <c r="B8" s="126"/>
       <c r="C8" s="46" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D8" s="102" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E8" s="27"/>
       <c r="F8" s="27" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G8" s="78"/>
       <c r="H8" s="72" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I8" s="42"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="129">
+      <c r="A9" s="118">
         <v>13</v>
       </c>
-      <c r="B9" s="131"/>
+      <c r="B9" s="126"/>
       <c r="C9" s="18">
         <f>I7 + 1</f>
         <v>9</v>
@@ -2061,20 +2068,20 @@
     </row>
     <row r="10" spans="1:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="119"/>
-      <c r="B10" s="131"/>
+      <c r="B10" s="126"/>
       <c r="C10" s="46" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D10" s="72" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E10" s="15"/>
       <c r="F10" s="14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G10" s="15"/>
       <c r="H10" s="16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I10" s="17"/>
     </row>
@@ -2082,7 +2089,7 @@
       <c r="A11" s="119">
         <v>12</v>
       </c>
-      <c r="B11" s="131"/>
+      <c r="B11" s="126"/>
       <c r="C11" s="21">
         <f>I9 + 1</f>
         <v>16</v>
@@ -2114,18 +2121,18 @@
     </row>
     <row r="12" spans="1:9" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="119"/>
-      <c r="B12" s="131"/>
+      <c r="B12" s="126"/>
       <c r="C12" s="43"/>
       <c r="D12" s="37" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E12" s="15"/>
       <c r="F12" s="27" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G12" s="15"/>
       <c r="H12" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I12" s="85"/>
     </row>
@@ -2133,7 +2140,7 @@
       <c r="A13" s="119">
         <v>11</v>
       </c>
-      <c r="B13" s="131"/>
+      <c r="B13" s="126"/>
       <c r="C13" s="21">
         <f>I11 + 1</f>
         <v>23</v>
@@ -2164,30 +2171,30 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="97.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="120"/>
-      <c r="B14" s="131"/>
+      <c r="A14" s="122"/>
+      <c r="B14" s="126"/>
       <c r="C14" s="43"/>
       <c r="D14" s="102" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E14" s="87"/>
       <c r="F14" s="40" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G14" s="100"/>
       <c r="H14" s="105" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I14" s="57" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="121">
+      <c r="A15" s="120">
         <v>10</v>
       </c>
-      <c r="B15" s="130" t="s">
-        <v>13</v>
+      <c r="B15" s="125" t="s">
+        <v>12</v>
       </c>
       <c r="C15" s="49">
         <v>1</v>
@@ -2218,8 +2225,8 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="122"/>
-      <c r="B16" s="132"/>
+      <c r="A16" s="121"/>
+      <c r="B16" s="127"/>
       <c r="C16" s="54" t="str">
         <f>I14</f>
         <v>WINTER BREAK</v>
@@ -2245,7 +2252,7 @@
         <v>WINTER BREAK</v>
       </c>
       <c r="I16" s="107" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="35" customFormat="1" ht="21.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -2264,7 +2271,7 @@
       <c r="B18" s="31"/>
       <c r="D18" s="34"/>
       <c r="E18" s="70" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F18" s="34"/>
       <c r="G18" s="34"/>
@@ -2276,7 +2283,7 @@
       <c r="B19" s="36"/>
       <c r="D19" s="30"/>
       <c r="E19" s="64" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F19" s="30"/>
       <c r="G19" s="30"/>
@@ -2288,7 +2295,7 @@
       <c r="B20" s="31"/>
       <c r="D20" s="34"/>
       <c r="E20" s="65" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F20" s="34"/>
       <c r="G20" s="34"/>
@@ -2300,7 +2307,7 @@
       <c r="B21" s="31"/>
       <c r="D21" s="34"/>
       <c r="E21" s="66" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F21" s="34"/>
       <c r="G21" s="34"/>
@@ -2312,7 +2319,7 @@
       <c r="B22" s="31"/>
       <c r="D22" s="34"/>
       <c r="E22" s="67" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F22" s="34"/>
       <c r="G22" s="34"/>
@@ -2325,7 +2332,7 @@
       <c r="C23" s="62"/>
       <c r="D23" s="34"/>
       <c r="E23" s="68" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F23" s="34"/>
       <c r="G23" s="34"/>
@@ -2355,22 +2362,22 @@
       <c r="I25" s="30"/>
     </row>
     <row r="26" spans="1:9" s="32" customFormat="1" ht="57.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="125" t="str">
+      <c r="A26" s="114" t="str">
         <f>A1</f>
         <v>CS320: SW Engineering - Spring 2020 Schedule
-(as of 3-22-2020, subject to change)</v>
-      </c>
-      <c r="B26" s="126"/>
-      <c r="C26" s="126"/>
-      <c r="D26" s="126"/>
-      <c r="E26" s="126"/>
-      <c r="F26" s="126"/>
-      <c r="G26" s="126"/>
-      <c r="H26" s="126"/>
-      <c r="I26" s="127"/>
+(as of 4-7-2020, subject to change)</v>
+      </c>
+      <c r="B26" s="115"/>
+      <c r="C26" s="115"/>
+      <c r="D26" s="115"/>
+      <c r="E26" s="115"/>
+      <c r="F26" s="115"/>
+      <c r="G26" s="115"/>
+      <c r="H26" s="115"/>
+      <c r="I26" s="116"/>
     </row>
     <row r="27" spans="1:9" s="2" customFormat="1" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="str">
+      <c r="A27" s="109" t="str">
         <f>A2</f>
         <v>Weeks</v>
       </c>
@@ -2405,7 +2412,7 @@
       </c>
     </row>
     <row r="28" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="128">
+      <c r="A28" s="117">
         <v>10</v>
       </c>
       <c r="B28" s="73"/>
@@ -2439,9 +2446,9 @@
       </c>
     </row>
     <row r="29" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="129"/>
-      <c r="B29" s="117" t="s">
-        <v>13</v>
+      <c r="A29" s="118"/>
+      <c r="B29" s="124" t="s">
+        <v>12</v>
       </c>
       <c r="C29" s="47" t="str">
         <f>C16</f>
@@ -2474,10 +2481,10 @@
       </c>
     </row>
     <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="129">
+      <c r="A30" s="118">
         <v>9</v>
       </c>
-      <c r="B30" s="117"/>
+      <c r="B30" s="124"/>
       <c r="C30" s="90">
         <f>I15 + 1</f>
         <v>8</v>
@@ -2509,31 +2516,31 @@
     </row>
     <row r="31" spans="1:9" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="119"/>
-      <c r="B31" s="117"/>
+      <c r="B31" s="124"/>
       <c r="C31" s="91" t="str">
         <f>H29</f>
         <v>WINTER BREAK</v>
       </c>
       <c r="D31" s="37" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E31" s="7"/>
       <c r="F31" s="24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G31" s="7"/>
       <c r="H31" s="102" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="I31" s="45" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="119">
         <v>8</v>
       </c>
-      <c r="B32" s="117"/>
+      <c r="B32" s="124"/>
       <c r="C32" s="25">
         <f>I30 + 1</f>
         <v>15</v>
@@ -2565,20 +2572,20 @@
     </row>
     <row r="33" spans="1:9" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="119"/>
-      <c r="B33" s="117"/>
+      <c r="B33" s="124"/>
       <c r="C33" s="10"/>
       <c r="D33" s="7" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="E33" s="28" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="G33" s="7"/>
       <c r="H33" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I33" s="71"/>
     </row>
@@ -2586,7 +2593,7 @@
       <c r="A34" s="119">
         <v>7</v>
       </c>
-      <c r="B34" s="117"/>
+      <c r="B34" s="124"/>
       <c r="C34" s="10">
         <f>I32 + 1</f>
         <v>22</v>
@@ -2618,20 +2625,20 @@
     </row>
     <row r="35" spans="1:9" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="119"/>
-      <c r="B35" s="117"/>
+      <c r="B35" s="124"/>
       <c r="C35" s="46" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E35" s="7"/>
       <c r="F35" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G35" s="7"/>
       <c r="H35" s="24" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I35" s="71"/>
     </row>
@@ -2669,32 +2676,32 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="69.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="122"/>
+      <c r="A37" s="121"/>
       <c r="B37" s="75"/>
       <c r="C37" s="111" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E37" s="104"/>
       <c r="F37" s="112" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="G37" s="27"/>
       <c r="H37" s="72" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I37" s="45" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="121">
+      <c r="A38" s="120">
         <v>5</v>
       </c>
-      <c r="B38" s="114" t="s">
-        <v>14</v>
+      <c r="B38" s="128" t="s">
+        <v>13</v>
       </c>
       <c r="C38" s="43">
         <f>I36 + 1</f>
@@ -2727,14 +2734,14 @@
     </row>
     <row r="39" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="119"/>
-      <c r="B39" s="115"/>
+      <c r="B39" s="129"/>
       <c r="C39" s="27"/>
       <c r="D39" s="113" t="s">
         <v>65</v>
       </c>
       <c r="E39" s="41"/>
       <c r="F39" s="37" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G39" s="60" t="s">
         <v>6</v>
@@ -2743,14 +2750,14 @@
         <v>6</v>
       </c>
       <c r="I39" s="45" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="119">
         <v>4</v>
       </c>
-      <c r="B40" s="115"/>
+      <c r="B40" s="129"/>
       <c r="C40" s="48">
         <f>I38 + 1</f>
         <v>12</v>
@@ -2782,7 +2789,7 @@
     </row>
     <row r="41" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="119"/>
-      <c r="B41" s="115"/>
+      <c r="B41" s="129"/>
       <c r="C41" s="47" t="s">
         <v>6</v>
       </c>
@@ -2791,11 +2798,11 @@
       </c>
       <c r="E41" s="15"/>
       <c r="F41" s="27" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="G41" s="27"/>
       <c r="H41" s="27" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
       <c r="I41" s="42"/>
     </row>
@@ -2803,7 +2810,7 @@
       <c r="A42" s="119">
         <v>3</v>
       </c>
-      <c r="B42" s="115"/>
+      <c r="B42" s="129"/>
       <c r="C42" s="43">
         <f>I40 + 1</f>
         <v>19</v>
@@ -2833,20 +2840,20 @@
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="119"/>
-      <c r="B43" s="115"/>
+      <c r="B43" s="129"/>
       <c r="C43" s="43"/>
-      <c r="D43" s="92" t="s">
-        <v>28</v>
+      <c r="D43" s="27" t="s">
+        <v>57</v>
       </c>
       <c r="E43" s="15"/>
-      <c r="F43" s="94" t="s">
-        <v>7</v>
+      <c r="F43" s="92" t="s">
+        <v>71</v>
       </c>
       <c r="G43" s="87"/>
       <c r="H43" s="94" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
       <c r="I43" s="85"/>
     </row>
@@ -2854,7 +2861,7 @@
       <c r="A44" s="119">
         <v>2</v>
       </c>
-      <c r="B44" s="115"/>
+      <c r="B44" s="129"/>
       <c r="C44" s="21">
         <f>I42 + 1</f>
         <v>26</v>
@@ -2883,28 +2890,28 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="122"/>
-      <c r="B45" s="115"/>
+    <row r="45" spans="1:9" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="121"/>
+      <c r="B45" s="129"/>
       <c r="C45" s="95"/>
       <c r="D45" s="105" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="E45" s="100"/>
       <c r="F45" s="105" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
       <c r="G45" s="103"/>
       <c r="H45" s="24" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
       <c r="I45" s="9"/>
     </row>
     <row r="46" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="121">
+      <c r="A46" s="120">
         <v>1</v>
       </c>
-      <c r="B46" s="116" t="s">
+      <c r="B46" s="123" t="s">
         <v>5</v>
       </c>
       <c r="C46" s="38">
@@ -2938,28 +2945,28 @@
     </row>
     <row r="47" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="119"/>
-      <c r="B47" s="117"/>
+      <c r="B47" s="124"/>
       <c r="C47" s="39"/>
       <c r="D47" s="7" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
       <c r="E47" s="44"/>
       <c r="F47" s="7" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
       <c r="G47" s="44"/>
       <c r="H47" s="108" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="I47" s="45" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="123" t="s">
-        <v>41</v>
-      </c>
-      <c r="B48" s="117"/>
+      <c r="A48" s="131" t="s">
+        <v>37</v>
+      </c>
+      <c r="B48" s="124"/>
       <c r="C48" s="25">
         <f>I46 + 1</f>
         <v>10</v>
@@ -2989,18 +2996,18 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="144" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="124"/>
-      <c r="B49" s="118"/>
+    <row r="49" spans="1:9" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="132"/>
+      <c r="B49" s="130"/>
       <c r="C49" s="69" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D49" s="29" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="E49" s="26"/>
       <c r="F49" s="29" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="G49" s="26"/>
       <c r="H49" s="12"/>
@@ -3009,6 +3016,19 @@
     <row r="50" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="B38:B45"/>
+    <mergeCell ref="B46:B49"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A40:A41"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A28:A29"/>
     <mergeCell ref="A30:A31"/>
@@ -3022,19 +3042,6 @@
     <mergeCell ref="A26:I26"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="B29:B35"/>
-    <mergeCell ref="B38:B45"/>
-    <mergeCell ref="B46:B49"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A40:A41"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated section 101 final pres time
</commit_message>
<xml_diff>
--- a/CS320-Spring2020Calendar.xlsx
+++ b/CS320-Spring2020Calendar.xlsx
@@ -380,10 +380,6 @@
  (Marmoset)</t>
   </si>
   <si>
-    <t>CS320: SW Engineering - Spring 2020 Schedule
-(as of 4-7-2020, subject to change)</t>
-  </si>
-  <si>
     <t>Team Project Work Session
 (Zoom)</t>
   </si>
@@ -437,12 +433,6 @@
 (Zoom)</t>
   </si>
   <si>
-    <t>FINAL EXAM PERIOD
-101: 8:00-10:00 102: 10:15-12:15
-A08: Team Presentation and Demonstration
-(Zoom)</t>
-  </si>
-  <si>
     <t>A03: Team MS2
 50% Progress on Features
 (Zoom)</t>
@@ -456,6 +446,16 @@
     <t>A03: Team MS3
 75% Working System (SQL DB)
 (Zoom)</t>
+  </si>
+  <si>
+    <t>FINAL EXAM PERIOD
+101: 9:00-10:00 102: 10:15-12:15
+A08: Team Presentation and Demonstration
+(Zoom)</t>
+  </si>
+  <si>
+    <t>CS320: SW Engineering - Spring 2020 Schedule
+(as of 5-6-2020, subject to change)</t>
   </si>
 </sst>
 </file>
@@ -1445,32 +1445,11 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -1478,6 +1457,42 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1485,21 +1500,6 @@
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1811,8 +1811,8 @@
   </sheetPr>
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1830,17 +1830,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="57.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="114" t="s">
-        <v>56</v>
-      </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
-      <c r="G1" s="115"/>
-      <c r="H1" s="115"/>
-      <c r="I1" s="116"/>
+      <c r="A1" s="125" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="126"/>
+      <c r="C1" s="126"/>
+      <c r="D1" s="126"/>
+      <c r="E1" s="126"/>
+      <c r="F1" s="126"/>
+      <c r="G1" s="126"/>
+      <c r="H1" s="126"/>
+      <c r="I1" s="127"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="109" t="s">
@@ -1870,10 +1870,10 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="120">
+      <c r="A3" s="121">
         <v>16</v>
       </c>
-      <c r="B3" s="123" t="s">
+      <c r="B3" s="116" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="49">
@@ -1906,7 +1906,7 @@
     </row>
     <row r="4" spans="1:9" ht="70.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="119"/>
-      <c r="B4" s="124"/>
+      <c r="B4" s="117"/>
       <c r="C4" s="47" t="s">
         <v>7</v>
       </c>
@@ -1929,7 +1929,7 @@
       <c r="A5" s="119">
         <v>15</v>
       </c>
-      <c r="B5" s="124"/>
+      <c r="B5" s="117"/>
       <c r="C5" s="10">
         <f>I3 + 1</f>
         <v>26</v>
@@ -1959,8 +1959,8 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="90.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="121"/>
-      <c r="B6" s="124"/>
+      <c r="A6" s="122"/>
+      <c r="B6" s="117"/>
       <c r="C6" s="79" t="s">
         <v>46</v>
       </c>
@@ -1978,10 +1978,10 @@
       <c r="I6" s="110"/>
     </row>
     <row r="7" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="120">
+      <c r="A7" s="121">
         <v>14</v>
       </c>
-      <c r="B7" s="125" t="s">
+      <c r="B7" s="130" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="82">
@@ -2014,8 +2014,8 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="122"/>
-      <c r="B8" s="126"/>
+      <c r="A8" s="120"/>
+      <c r="B8" s="131"/>
       <c r="C8" s="46" t="s">
         <v>48</v>
       </c>
@@ -2033,10 +2033,10 @@
       <c r="I8" s="42"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="118">
+      <c r="A9" s="129">
         <v>13</v>
       </c>
-      <c r="B9" s="126"/>
+      <c r="B9" s="131"/>
       <c r="C9" s="18">
         <f>I7 + 1</f>
         <v>9</v>
@@ -2068,7 +2068,7 @@
     </row>
     <row r="10" spans="1:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="119"/>
-      <c r="B10" s="126"/>
+      <c r="B10" s="131"/>
       <c r="C10" s="46" t="s">
         <v>49</v>
       </c>
@@ -2089,7 +2089,7 @@
       <c r="A11" s="119">
         <v>12</v>
       </c>
-      <c r="B11" s="126"/>
+      <c r="B11" s="131"/>
       <c r="C11" s="21">
         <f>I9 + 1</f>
         <v>16</v>
@@ -2121,7 +2121,7 @@
     </row>
     <row r="12" spans="1:9" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="119"/>
-      <c r="B12" s="126"/>
+      <c r="B12" s="131"/>
       <c r="C12" s="43"/>
       <c r="D12" s="37" t="s">
         <v>27</v>
@@ -2140,7 +2140,7 @@
       <c r="A13" s="119">
         <v>11</v>
       </c>
-      <c r="B13" s="126"/>
+      <c r="B13" s="131"/>
       <c r="C13" s="21">
         <f>I11 + 1</f>
         <v>23</v>
@@ -2171,8 +2171,8 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="97.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="122"/>
-      <c r="B14" s="126"/>
+      <c r="A14" s="120"/>
+      <c r="B14" s="131"/>
       <c r="C14" s="43"/>
       <c r="D14" s="102" t="s">
         <v>39</v>
@@ -2190,10 +2190,10 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="120">
+      <c r="A15" s="121">
         <v>10</v>
       </c>
-      <c r="B15" s="125" t="s">
+      <c r="B15" s="130" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="49">
@@ -2225,8 +2225,8 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="121"/>
-      <c r="B16" s="127"/>
+      <c r="A16" s="122"/>
+      <c r="B16" s="132"/>
       <c r="C16" s="54" t="str">
         <f>I14</f>
         <v>WINTER BREAK</v>
@@ -2362,19 +2362,19 @@
       <c r="I25" s="30"/>
     </row>
     <row r="26" spans="1:9" s="32" customFormat="1" ht="57.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="114" t="str">
+      <c r="A26" s="125" t="str">
         <f>A1</f>
         <v>CS320: SW Engineering - Spring 2020 Schedule
-(as of 4-7-2020, subject to change)</v>
-      </c>
-      <c r="B26" s="115"/>
-      <c r="C26" s="115"/>
-      <c r="D26" s="115"/>
-      <c r="E26" s="115"/>
-      <c r="F26" s="115"/>
-      <c r="G26" s="115"/>
-      <c r="H26" s="115"/>
-      <c r="I26" s="116"/>
+(as of 5-6-2020, subject to change)</v>
+      </c>
+      <c r="B26" s="126"/>
+      <c r="C26" s="126"/>
+      <c r="D26" s="126"/>
+      <c r="E26" s="126"/>
+      <c r="F26" s="126"/>
+      <c r="G26" s="126"/>
+      <c r="H26" s="126"/>
+      <c r="I26" s="127"/>
     </row>
     <row r="27" spans="1:9" s="2" customFormat="1" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="109" t="str">
@@ -2412,7 +2412,7 @@
       </c>
     </row>
     <row r="28" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="117">
+      <c r="A28" s="128">
         <v>10</v>
       </c>
       <c r="B28" s="73"/>
@@ -2446,8 +2446,8 @@
       </c>
     </row>
     <row r="29" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="118"/>
-      <c r="B29" s="124" t="s">
+      <c r="A29" s="129"/>
+      <c r="B29" s="117" t="s">
         <v>12</v>
       </c>
       <c r="C29" s="47" t="str">
@@ -2481,10 +2481,10 @@
       </c>
     </row>
     <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="118">
+      <c r="A30" s="129">
         <v>9</v>
       </c>
-      <c r="B30" s="124"/>
+      <c r="B30" s="117"/>
       <c r="C30" s="90">
         <f>I15 + 1</f>
         <v>8</v>
@@ -2516,7 +2516,7 @@
     </row>
     <row r="31" spans="1:9" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="119"/>
-      <c r="B31" s="124"/>
+      <c r="B31" s="117"/>
       <c r="C31" s="91" t="str">
         <f>H29</f>
         <v>WINTER BREAK</v>
@@ -2540,7 +2540,7 @@
       <c r="A32" s="119">
         <v>8</v>
       </c>
-      <c r="B32" s="124"/>
+      <c r="B32" s="117"/>
       <c r="C32" s="25">
         <f>I30 + 1</f>
         <v>15</v>
@@ -2572,20 +2572,20 @@
     </row>
     <row r="33" spans="1:9" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="119"/>
-      <c r="B33" s="124"/>
+      <c r="B33" s="117"/>
       <c r="C33" s="10"/>
       <c r="D33" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E33" s="28" t="s">
         <v>53</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G33" s="7"/>
       <c r="H33" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I33" s="71"/>
     </row>
@@ -2593,7 +2593,7 @@
       <c r="A34" s="119">
         <v>7</v>
       </c>
-      <c r="B34" s="124"/>
+      <c r="B34" s="117"/>
       <c r="C34" s="10">
         <f>I32 + 1</f>
         <v>22</v>
@@ -2625,20 +2625,20 @@
     </row>
     <row r="35" spans="1:9" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="119"/>
-      <c r="B35" s="124"/>
+      <c r="B35" s="117"/>
       <c r="C35" s="46" t="s">
         <v>34</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E35" s="7"/>
       <c r="F35" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G35" s="7"/>
       <c r="H35" s="24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I35" s="71"/>
     </row>
@@ -2676,31 +2676,31 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="69.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="121"/>
+      <c r="A37" s="122"/>
       <c r="B37" s="75"/>
       <c r="C37" s="111" t="s">
         <v>55</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E37" s="104"/>
       <c r="F37" s="112" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G37" s="27"/>
       <c r="H37" s="72" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I37" s="45" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="120">
+      <c r="A38" s="121">
         <v>5</v>
       </c>
-      <c r="B38" s="128" t="s">
+      <c r="B38" s="114" t="s">
         <v>13</v>
       </c>
       <c r="C38" s="43">
@@ -2734,14 +2734,14 @@
     </row>
     <row r="39" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="119"/>
-      <c r="B39" s="129"/>
+      <c r="B39" s="115"/>
       <c r="C39" s="27"/>
       <c r="D39" s="113" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E39" s="41"/>
       <c r="F39" s="37" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G39" s="60" t="s">
         <v>6</v>
@@ -2757,7 +2757,7 @@
       <c r="A40" s="119">
         <v>4</v>
       </c>
-      <c r="B40" s="129"/>
+      <c r="B40" s="115"/>
       <c r="C40" s="48">
         <f>I38 + 1</f>
         <v>12</v>
@@ -2789,7 +2789,7 @@
     </row>
     <row r="41" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="119"/>
-      <c r="B41" s="129"/>
+      <c r="B41" s="115"/>
       <c r="C41" s="47" t="s">
         <v>6</v>
       </c>
@@ -2798,11 +2798,11 @@
       </c>
       <c r="E41" s="15"/>
       <c r="F41" s="27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G41" s="27"/>
       <c r="H41" s="27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I41" s="42"/>
     </row>
@@ -2810,7 +2810,7 @@
       <c r="A42" s="119">
         <v>3</v>
       </c>
-      <c r="B42" s="129"/>
+      <c r="B42" s="115"/>
       <c r="C42" s="43">
         <f>I40 + 1</f>
         <v>19</v>
@@ -2842,18 +2842,18 @@
     </row>
     <row r="43" spans="1:9" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="119"/>
-      <c r="B43" s="129"/>
+      <c r="B43" s="115"/>
       <c r="C43" s="43"/>
       <c r="D43" s="27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E43" s="15"/>
       <c r="F43" s="92" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G43" s="87"/>
       <c r="H43" s="94" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I43" s="85"/>
     </row>
@@ -2861,7 +2861,7 @@
       <c r="A44" s="119">
         <v>2</v>
       </c>
-      <c r="B44" s="129"/>
+      <c r="B44" s="115"/>
       <c r="C44" s="21">
         <f>I42 + 1</f>
         <v>26</v>
@@ -2891,27 +2891,27 @@
       </c>
     </row>
     <row r="45" spans="1:9" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="121"/>
-      <c r="B45" s="129"/>
+      <c r="A45" s="122"/>
+      <c r="B45" s="115"/>
       <c r="C45" s="95"/>
       <c r="D45" s="105" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E45" s="100"/>
       <c r="F45" s="105" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G45" s="103"/>
       <c r="H45" s="24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I45" s="9"/>
     </row>
     <row r="46" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="120">
+      <c r="A46" s="121">
         <v>1</v>
       </c>
-      <c r="B46" s="123" t="s">
+      <c r="B46" s="116" t="s">
         <v>5</v>
       </c>
       <c r="C46" s="38">
@@ -2945,14 +2945,14 @@
     </row>
     <row r="47" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="119"/>
-      <c r="B47" s="124"/>
+      <c r="B47" s="117"/>
       <c r="C47" s="39"/>
       <c r="D47" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E47" s="44"/>
       <c r="F47" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G47" s="44"/>
       <c r="H47" s="108" t="s">
@@ -2963,10 +2963,10 @@
       </c>
     </row>
     <row r="48" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="131" t="s">
+      <c r="A48" s="123" t="s">
         <v>37</v>
       </c>
-      <c r="B48" s="124"/>
+      <c r="B48" s="117"/>
       <c r="C48" s="25">
         <f>I46 + 1</f>
         <v>10</v>
@@ -2997,17 +2997,17 @@
       </c>
     </row>
     <row r="49" spans="1:9" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="132"/>
-      <c r="B49" s="130"/>
+      <c r="A49" s="124"/>
+      <c r="B49" s="118"/>
       <c r="C49" s="69" t="s">
         <v>36</v>
       </c>
       <c r="D49" s="29" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E49" s="26"/>
       <c r="F49" s="29" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G49" s="26"/>
       <c r="H49" s="12"/>
@@ -3016,6 +3016,19 @@
     <row r="50" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="B7:B14"/>
+    <mergeCell ref="A26:I26"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B29:B35"/>
     <mergeCell ref="B38:B45"/>
     <mergeCell ref="B46:B49"/>
     <mergeCell ref="A13:A14"/>
@@ -3029,19 +3042,6 @@
     <mergeCell ref="A36:A37"/>
     <mergeCell ref="A38:A39"/>
     <mergeCell ref="A40:A41"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="B7:B14"/>
-    <mergeCell ref="A26:I26"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B29:B35"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>